<commit_message>
Finnish language, release candidate.
</commit_message>
<xml_diff>
--- a/Documentation/translation.xlsx
+++ b/Documentation/translation.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2269" uniqueCount="1731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="1751">
   <si>
     <t>$this.Text</t>
   </si>
@@ -4420,9 +4420,6 @@
     <t>Lisätietoja ohjelmasta Wake On LAN</t>
   </si>
   <si>
-    <t>lähiverkossa hätätapauksessa.</t>
-  </si>
-  <si>
     <t>Peruuta sammutus</t>
   </si>
   <si>
@@ -4459,9 +4456,6 @@
     <t>Poistu</t>
   </si>
   <si>
-    <t>Vie</t>
-  </si>
-  <si>
     <t>Tiedosto</t>
   </si>
   <si>
@@ -5210,13 +5204,79 @@
   </si>
   <si>
     <t>[Listener]</t>
+  </si>
+  <si>
+    <t>Lähettää "magic pakets" -komentoja Ethernet-korteille "herättääkseen" tietokoneet etänä. Sulje tietokoneita etänä. Suorita "yleinen hätäsammutus" kaikille LAN-verkkoon kytketyille tietokoneille.</t>
+  </si>
+  <si>
+    <t>Vie (tallenna)</t>
+  </si>
+  <si>
+    <t>klo {0} joka {1}</t>
+  </si>
+  <si>
+    <t>klo {0} joka {1} päivä</t>
+  </si>
+  <si>
+    <t>klo {0} joka {2} viikon {1}, alkaen {3}</t>
+  </si>
+  <si>
+    <t>Väärä</t>
+  </si>
+  <si>
+    <t>Useita laukaisimia määritelty</t>
+  </si>
+  <si>
+    <t>Hae päivityksiä automaattisesti</t>
+  </si>
+  <si>
+    <t>Palauta oletukset</t>
+  </si>
+  <si>
+    <t>Verkko-/käyttäjätunnus</t>
+  </si>
+  <si>
+    <t>Palauta oletu</t>
+  </si>
+  <si>
+    <t>Laske aliverkko</t>
+  </si>
+  <si>
+    <t>Tämä toiminto auttaa sinua löytämään IP- ja aliverkko-osoitteen avulla käytettävän ”Broadcast osoitteen.”</t>
+  </si>
+  <si>
+    <t>Suositeltu ”Broadcast osoite:”</t>
+  </si>
+  <si>
+    <t>Aliverkko</t>
+  </si>
+  <si>
+    <t>Kuuntelija</t>
+  </si>
+  <si>
+    <t>Tyhjennä</t>
+  </si>
+  <si>
+    <t>Aika</t>
+  </si>
+  <si>
+    <t>Verkkoasetukset</t>
+  </si>
+  <si>
+    <t>UDP-portti 9</t>
+  </si>
+  <si>
+    <t>WakeOnLAN -paketteja vastaanotettu...</t>
+  </si>
+  <si>
+    <t>Kuuntelee:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5272,13 +5332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -5313,19 +5366,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5335,11 +5389,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -5354,6 +5403,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="34"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5364,15 +5425,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5401,26 +5463,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5431,14 +5477,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="5"/>
-    <cellStyle name="Excel Built-in Normal" xfId="4"/>
+  <cellStyles count="7">
+    <cellStyle name="Excel Built-in Bad" xfId="6"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="4"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Excel Built-in Normal 1" xfId="5"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5740,8 +5800,8 @@
   <dimension ref="A1:XFD379"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5749,7 +5809,7 @@
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" customWidth="1"/>
     <col min="5" max="5" width="58.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.42578125" style="3" customWidth="1"/>
     <col min="7" max="10" width="36.7109375" customWidth="1"/>
@@ -5765,7 +5825,7 @@
       <c r="C1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="24" t="s">
         <v>1462</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -5804,7 +5864,7 @@
       <c r="C3" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="24" t="s">
         <v>1463</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -5827,7 +5887,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="18"/>
+      <c r="D4" s="24"/>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5844,7 +5904,7 @@
       <c r="C6" t="s">
         <v>310</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="25" t="s">
         <v>310</v>
       </c>
       <c r="E6" t="s">
@@ -5873,7 +5933,7 @@
       <c r="C7" t="s">
         <v>311</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="25" t="s">
         <v>1464</v>
       </c>
       <c r="E7" t="s">
@@ -5903,7 +5963,7 @@
       <c r="C8" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="25" t="s">
         <v>1465</v>
       </c>
       <c r="E8" t="s">
@@ -5918,13 +5978,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>753</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="25" t="s">
         <v>1465</v>
       </c>
       <c r="E9" t="s">
@@ -5990,7 +6050,7 @@
       <c r="C14" t="s">
         <v>312</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="25" t="s">
         <v>1466</v>
       </c>
       <c r="E14" t="s">
@@ -6013,11 +6073,11 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>1467</v>
+      <c r="D15" t="s">
+        <v>1729</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -6049,8 +6109,8 @@
       <c r="C18" t="s">
         <v>314</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>1468</v>
+      <c r="D18" s="25" t="s">
+        <v>1467</v>
       </c>
       <c r="E18" t="s">
         <v>1241</v>
@@ -6075,8 +6135,8 @@
       <c r="C19" t="s">
         <v>315</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>1469</v>
+      <c r="D19" s="25" t="s">
+        <v>1468</v>
       </c>
       <c r="E19" t="s">
         <v>1242</v>
@@ -6101,8 +6161,8 @@
       <c r="C20" t="s">
         <v>316</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>1470</v>
+      <c r="D20" s="25" t="s">
+        <v>1469</v>
       </c>
       <c r="E20" t="s">
         <v>1243</v>
@@ -6127,8 +6187,8 @@
       <c r="C21" t="s">
         <v>323</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>1471</v>
+      <c r="D21" s="25" t="s">
+        <v>1470</v>
       </c>
       <c r="E21" t="s">
         <v>1244</v>
@@ -6153,8 +6213,8 @@
       <c r="C22" t="s">
         <v>317</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>1472</v>
+      <c r="D22" s="25" t="s">
+        <v>1471</v>
       </c>
       <c r="E22" t="s">
         <v>1245</v>
@@ -6179,8 +6239,8 @@
       <c r="C23" t="s">
         <v>322</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>1473</v>
+      <c r="D23" s="25" t="s">
+        <v>1472</v>
       </c>
       <c r="E23" t="s">
         <v>1246</v>
@@ -6208,8 +6268,8 @@
       <c r="C24" t="s">
         <v>1192</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>1474</v>
+      <c r="D24" s="25" t="s">
+        <v>1473</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -6234,8 +6294,8 @@
       <c r="C25" t="s">
         <v>325</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>1475</v>
+      <c r="D25" s="25" t="s">
+        <v>1474</v>
       </c>
       <c r="E25" t="s">
         <v>206</v>
@@ -6260,8 +6320,8 @@
       <c r="C26" t="s">
         <v>324</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>1476</v>
+      <c r="D26" s="25" t="s">
+        <v>1475</v>
       </c>
       <c r="E26" t="s">
         <v>1247</v>
@@ -6286,8 +6346,8 @@
       <c r="C27" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>1477</v>
+      <c r="D27" s="25" t="s">
+        <v>1476</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -6312,8 +6372,8 @@
       <c r="C28" t="s">
         <v>326</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>1478</v>
+      <c r="D28" s="25" t="s">
+        <v>1477</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
@@ -6341,8 +6401,8 @@
       <c r="C29" t="s">
         <v>1175</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>1479</v>
+      <c r="D29" s="25" t="s">
+        <v>1478</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
@@ -6370,8 +6430,8 @@
       <c r="C30" t="s">
         <v>1193</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>1480</v>
+      <c r="D30" s="25" t="s">
+        <v>1730</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
@@ -6396,8 +6456,8 @@
       <c r="C31" t="s">
         <v>327</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>1481</v>
+      <c r="D31" s="25" t="s">
+        <v>1479</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -6422,8 +6482,8 @@
       <c r="C32" t="s">
         <v>328</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>1482</v>
+      <c r="D32" s="25" t="s">
+        <v>1480</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -6449,8 +6509,8 @@
       <c r="C33" s="9" t="s">
         <v>876</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>1483</v>
+      <c r="D33" s="26" t="s">
+        <v>1481</v>
       </c>
       <c r="E33" t="s">
         <v>1248</v>
@@ -6469,8 +6529,8 @@
       <c r="C34" t="s">
         <v>328</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>1482</v>
+      <c r="D34" s="25" t="s">
+        <v>1480</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
@@ -6495,8 +6555,8 @@
       <c r="C35" t="s">
         <v>329</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>1484</v>
+      <c r="D35" s="25" t="s">
+        <v>1482</v>
       </c>
       <c r="E35" t="s">
         <v>28</v>
@@ -6524,8 +6584,8 @@
       <c r="C36" t="s">
         <v>1194</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>1485</v>
+      <c r="D36" s="25" t="s">
+        <v>1483</v>
       </c>
       <c r="E36" t="s">
         <v>30</v>
@@ -6543,32 +6603,32 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+    <row r="37" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="18" t="s">
         <v>1222</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="18" t="s">
         <v>1160</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>1486</v>
-      </c>
-      <c r="E37" s="25" t="s">
+      <c r="D37" s="27" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="19" t="s">
         <v>1160</v>
       </c>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="18" t="s">
         <v>630</v>
       </c>
-      <c r="H37" s="25" t="s">
+      <c r="H37" s="18" t="s">
         <v>596</v>
       </c>
-      <c r="I37" s="25" t="s">
+      <c r="I37" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6579,8 +6639,8 @@
       <c r="C38" t="s">
         <v>330</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>1487</v>
+      <c r="D38" s="25" t="s">
+        <v>1485</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
@@ -6605,8 +6665,8 @@
       <c r="C39" t="s">
         <v>331</v>
       </c>
-      <c r="D39" s="17" t="s">
-        <v>1488</v>
+      <c r="D39" s="25" t="s">
+        <v>1486</v>
       </c>
       <c r="E39" t="s">
         <v>1249</v>
@@ -6632,8 +6692,8 @@
       <c r="C40" s="9" t="s">
         <v>884</v>
       </c>
-      <c r="D40" s="21" t="s">
-        <v>1489</v>
+      <c r="D40" s="26" t="s">
+        <v>1487</v>
       </c>
       <c r="E40" t="s">
         <v>1250</v>
@@ -6652,8 +6712,8 @@
       <c r="C41" t="s">
         <v>332</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>1490</v>
+      <c r="D41" s="25" t="s">
+        <v>1488</v>
       </c>
       <c r="E41" t="s">
         <v>38</v>
@@ -6678,8 +6738,8 @@
       <c r="C42" t="s">
         <v>333</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>1491</v>
+      <c r="D42" s="25" t="s">
+        <v>1489</v>
       </c>
       <c r="E42" t="s">
         <v>1251</v>
@@ -6707,8 +6767,8 @@
       <c r="C43" t="s">
         <v>240</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>1492</v>
+      <c r="D43" s="25" t="s">
+        <v>1490</v>
       </c>
       <c r="E43" t="s">
         <v>1252</v>
@@ -6733,8 +6793,8 @@
       <c r="C44" t="s">
         <v>334</v>
       </c>
-      <c r="D44" s="17" t="s">
-        <v>1493</v>
+      <c r="D44" s="25" t="s">
+        <v>1682</v>
       </c>
       <c r="E44" t="s">
         <v>44</v>
@@ -6759,8 +6819,8 @@
       <c r="C45" t="s">
         <v>335</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>1494</v>
+      <c r="D45" s="25" t="s">
+        <v>1492</v>
       </c>
       <c r="E45" t="s">
         <v>210</v>
@@ -6785,8 +6845,8 @@
       <c r="C46" t="s">
         <v>874</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>1495</v>
+      <c r="D46" s="25" t="s">
+        <v>1493</v>
       </c>
       <c r="E46" t="s">
         <v>46</v>
@@ -6811,8 +6871,8 @@
       <c r="C47" t="s">
         <v>1196</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>1496</v>
+      <c r="D47" s="25" t="s">
+        <v>1494</v>
       </c>
       <c r="E47" t="s">
         <v>212</v>
@@ -6837,8 +6897,8 @@
       <c r="C48" t="s">
         <v>1197</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>1497</v>
+      <c r="D48" s="25" t="s">
+        <v>1495</v>
       </c>
       <c r="E48" t="s">
         <v>212</v>
@@ -6863,8 +6923,8 @@
       <c r="C49" t="s">
         <v>173</v>
       </c>
-      <c r="D49" s="17" t="s">
-        <v>1498</v>
+      <c r="D49" s="25" t="s">
+        <v>1496</v>
       </c>
       <c r="E49" t="s">
         <v>48</v>
@@ -6892,8 +6952,8 @@
       <c r="C50" t="s">
         <v>1199</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>1499</v>
+      <c r="D50" s="25" t="s">
+        <v>1497</v>
       </c>
       <c r="E50" t="s">
         <v>50</v>
@@ -6918,8 +6978,8 @@
       <c r="C51" t="s">
         <v>1200</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>1500</v>
+      <c r="D51" s="25" t="s">
+        <v>1498</v>
       </c>
       <c r="E51" t="s">
         <v>215</v>
@@ -6944,8 +7004,8 @@
       <c r="C52" t="s">
         <v>337</v>
       </c>
-      <c r="D52" s="17" t="s">
-        <v>1501</v>
+      <c r="D52" s="25" t="s">
+        <v>1499</v>
       </c>
       <c r="E52" t="s">
         <v>36</v>
@@ -6970,8 +7030,8 @@
       <c r="C53" t="s">
         <v>338</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>1502</v>
+      <c r="D53" s="25" t="s">
+        <v>1500</v>
       </c>
       <c r="E53" t="s">
         <v>1253</v>
@@ -6996,8 +7056,8 @@
       <c r="C54" t="s">
         <v>1201</v>
       </c>
-      <c r="D54" s="17" t="s">
-        <v>1503</v>
+      <c r="D54" s="25" t="s">
+        <v>1501</v>
       </c>
       <c r="E54" t="s">
         <v>55</v>
@@ -7022,8 +7082,8 @@
       <c r="C55" t="s">
         <v>1202</v>
       </c>
-      <c r="D55" s="17" t="s">
-        <v>1504</v>
+      <c r="D55" s="25" t="s">
+        <v>1502</v>
       </c>
       <c r="E55" t="s">
         <v>1254</v>
@@ -7048,8 +7108,8 @@
       <c r="C56" t="s">
         <v>339</v>
       </c>
-      <c r="D56" s="17" t="s">
-        <v>1505</v>
+      <c r="D56" s="25" t="s">
+        <v>1503</v>
       </c>
       <c r="E56" t="s">
         <v>1255</v>
@@ -7074,8 +7134,8 @@
       <c r="C57" t="s">
         <v>340</v>
       </c>
-      <c r="D57" s="17" t="s">
-        <v>1506</v>
+      <c r="D57" s="25" t="s">
+        <v>1504</v>
       </c>
       <c r="E57" t="s">
         <v>1256</v>
@@ -7101,8 +7161,8 @@
       <c r="C58" t="s">
         <v>341</v>
       </c>
-      <c r="D58" s="17" t="s">
-        <v>1507</v>
+      <c r="D58" s="25" t="s">
+        <v>1505</v>
       </c>
       <c r="E58" t="s">
         <v>1257</v>
@@ -7127,8 +7187,8 @@
       <c r="C59" t="s">
         <v>342</v>
       </c>
-      <c r="D59" s="17" t="s">
-        <v>1508</v>
+      <c r="D59" s="25" t="s">
+        <v>1506</v>
       </c>
       <c r="E59" t="s">
         <v>1258</v>
@@ -7154,8 +7214,8 @@
       <c r="C60" t="s">
         <v>1203</v>
       </c>
-      <c r="D60" s="17" t="s">
-        <v>1509</v>
+      <c r="D60" s="25" t="s">
+        <v>1507</v>
       </c>
       <c r="E60" t="s">
         <v>1259</v>
@@ -7180,8 +7240,8 @@
       <c r="C61" t="s">
         <v>650</v>
       </c>
-      <c r="D61" s="17" t="s">
-        <v>1510</v>
+      <c r="D61" s="25" t="s">
+        <v>1508</v>
       </c>
       <c r="E61" t="s">
         <v>65</v>
@@ -7206,8 +7266,8 @@
       <c r="C62" t="s">
         <v>1204</v>
       </c>
-      <c r="D62" s="17" t="s">
-        <v>1511</v>
+      <c r="D62" s="25" t="s">
+        <v>1509</v>
       </c>
       <c r="E62" t="s">
         <v>1260</v>
@@ -7232,8 +7292,8 @@
       <c r="C63" t="s">
         <v>1205</v>
       </c>
-      <c r="D63" s="17" t="s">
-        <v>1512</v>
+      <c r="D63" s="25" t="s">
+        <v>1510</v>
       </c>
       <c r="E63" t="s">
         <v>72</v>
@@ -7261,8 +7321,8 @@
       <c r="C64" t="s">
         <v>1206</v>
       </c>
-      <c r="D64" s="17" t="s">
-        <v>1513</v>
+      <c r="D64" s="25" t="s">
+        <v>1511</v>
       </c>
       <c r="E64" t="s">
         <v>1261</v>
@@ -7287,8 +7347,8 @@
       <c r="C65" t="s">
         <v>343</v>
       </c>
-      <c r="D65" s="17" t="s">
-        <v>1514</v>
+      <c r="D65" s="25" t="s">
+        <v>1512</v>
       </c>
       <c r="E65" t="s">
         <v>1262</v>
@@ -7314,8 +7374,8 @@
       <c r="C66" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="D66" s="22" t="s">
-        <v>1515</v>
+      <c r="D66" s="28" t="s">
+        <v>1513</v>
       </c>
       <c r="E66" t="s">
         <v>1444</v>
@@ -7338,8 +7398,8 @@
       <c r="C67" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="D67" s="22" t="s">
-        <v>1515</v>
+      <c r="D67" s="28" t="s">
+        <v>1513</v>
       </c>
       <c r="E67" t="s">
         <v>1444</v>
@@ -7362,7 +7422,7 @@
       <c r="C68" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="D68" s="22" t="s">
+      <c r="D68" s="28" t="s">
         <v>553</v>
       </c>
       <c r="E68" t="s">
@@ -7386,7 +7446,7 @@
       <c r="C69" s="6" t="s">
         <v>554</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D69" s="28" t="s">
         <v>555</v>
       </c>
       <c r="E69" t="s">
@@ -7410,8 +7470,8 @@
       <c r="C70" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="D70" s="22" t="s">
-        <v>1516</v>
+      <c r="D70" s="28" t="s">
+        <v>1514</v>
       </c>
       <c r="E70" t="s">
         <v>1265</v>
@@ -7434,8 +7494,8 @@
       <c r="C71" s="6" t="s">
         <v>558</v>
       </c>
-      <c r="D71" s="22" t="s">
-        <v>1517</v>
+      <c r="D71" s="28" t="s">
+        <v>1515</v>
       </c>
       <c r="E71" t="s">
         <v>1266</v>
@@ -7458,8 +7518,8 @@
       <c r="C72" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="D72" s="22" t="s">
-        <v>1518</v>
+      <c r="D72" s="28" t="s">
+        <v>1516</v>
       </c>
       <c r="E72" t="s">
         <v>1267</v>
@@ -7482,8 +7542,8 @@
       <c r="C73" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="D73" s="22" t="s">
-        <v>1519</v>
+      <c r="D73" s="28" t="s">
+        <v>1517</v>
       </c>
       <c r="E73" t="s">
         <v>1268</v>
@@ -7506,8 +7566,8 @@
       <c r="C74" s="6" t="s">
         <v>1166</v>
       </c>
-      <c r="D74" s="22" t="s">
-        <v>1520</v>
+      <c r="D74" s="28" t="s">
+        <v>1518</v>
       </c>
       <c r="E74" t="s">
         <v>1269</v>
@@ -7531,8 +7591,8 @@
       <c r="C75" s="6" t="s">
         <v>1170</v>
       </c>
-      <c r="D75" s="22" t="s">
-        <v>1521</v>
+      <c r="D75" s="28" t="s">
+        <v>1519</v>
       </c>
       <c r="E75" t="s">
         <v>1270</v>
@@ -7555,8 +7615,8 @@
       <c r="C76" t="s">
         <v>1173</v>
       </c>
-      <c r="D76" s="17" t="s">
-        <v>1522</v>
+      <c r="D76" s="25" t="s">
+        <v>1520</v>
       </c>
       <c r="E76" t="s">
         <v>1271</v>
@@ -7579,8 +7639,8 @@
       <c r="C77" t="s">
         <v>1175</v>
       </c>
-      <c r="D77" s="17" t="s">
-        <v>1479</v>
+      <c r="D77" s="25" t="s">
+        <v>1478</v>
       </c>
       <c r="E77" t="s">
         <v>1272</v>
@@ -7603,8 +7663,8 @@
       <c r="C78" s="6" t="s">
         <v>1176</v>
       </c>
-      <c r="D78" s="22" t="s">
-        <v>1523</v>
+      <c r="D78" s="28" t="s">
+        <v>1521</v>
       </c>
       <c r="E78" t="s">
         <v>1273</v>
@@ -7628,8 +7688,8 @@
       <c r="C79" s="3" t="s">
         <v>1436</v>
       </c>
-      <c r="D79" s="22" t="s">
-        <v>1524</v>
+      <c r="D79" s="28" t="s">
+        <v>1522</v>
       </c>
       <c r="E79" t="s">
         <v>1261</v>
@@ -7896,8 +7956,8 @@
       <c r="C80" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="D80" s="22" t="s">
-        <v>1525</v>
+      <c r="D80" s="28" t="s">
+        <v>1523</v>
       </c>
       <c r="E80" t="s">
         <v>1264</v>
@@ -8164,8 +8224,8 @@
       <c r="C81" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="D81" s="22" t="s">
-        <v>1526</v>
+      <c r="D81" s="28" t="s">
+        <v>1524</v>
       </c>
       <c r="E81" t="s">
         <v>1265</v>
@@ -8432,8 +8492,8 @@
       <c r="C82" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="D82" s="22" t="s">
-        <v>1517</v>
+      <c r="D82" s="28" t="s">
+        <v>1515</v>
       </c>
       <c r="E82" t="s">
         <v>1266</v>
@@ -8700,8 +8760,8 @@
       <c r="C83" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="D83" s="22" t="s">
-        <v>1518</v>
+      <c r="D83" s="28" t="s">
+        <v>1516</v>
       </c>
       <c r="E83" t="s">
         <v>1267</v>
@@ -8968,8 +9028,8 @@
       <c r="C84" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="D84" s="22" t="s">
-        <v>1519</v>
+      <c r="D84" s="28" t="s">
+        <v>1517</v>
       </c>
       <c r="E84" t="s">
         <v>1268</v>
@@ -9235,8 +9295,8 @@
       <c r="C85" s="3" t="s">
         <v>1443</v>
       </c>
-      <c r="D85" s="22" t="s">
-        <v>1527</v>
+      <c r="D85" s="28" t="s">
+        <v>1525</v>
       </c>
       <c r="E85" t="s">
         <v>1445</v>
@@ -9257,8 +9317,8 @@
       <c r="C88" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D88" s="19" t="s">
-        <v>1528</v>
+      <c r="D88" s="25" t="s">
+        <v>1526</v>
       </c>
       <c r="E88" t="s">
         <v>1274</v>
@@ -9281,8 +9341,8 @@
       <c r="C89" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="D89" s="19" t="s">
-        <v>1529</v>
+      <c r="D89" s="25" t="s">
+        <v>1527</v>
       </c>
       <c r="E89" t="s">
         <v>1275</v>
@@ -9305,8 +9365,8 @@
       <c r="C90" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="D90" s="19" t="s">
-        <v>1530</v>
+      <c r="D90" s="25" t="s">
+        <v>1528</v>
       </c>
       <c r="E90" t="s">
         <v>1276</v>
@@ -9336,8 +9396,8 @@
       <c r="C93" t="s">
         <v>173</v>
       </c>
-      <c r="D93" s="17" t="s">
-        <v>1498</v>
+      <c r="D93" s="25" t="s">
+        <v>1496</v>
       </c>
       <c r="E93" t="s">
         <v>48</v>
@@ -9359,8 +9419,8 @@
       <c r="C94" t="s">
         <v>344</v>
       </c>
-      <c r="D94" s="17" t="s">
-        <v>1531</v>
+      <c r="D94" s="25" t="s">
+        <v>1529</v>
       </c>
       <c r="E94" t="s">
         <v>1277</v>
@@ -9385,8 +9445,8 @@
       <c r="C95" t="s">
         <v>149</v>
       </c>
-      <c r="D95" s="17" t="s">
-        <v>1477</v>
+      <c r="D95" s="25" t="s">
+        <v>1476</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -9411,8 +9471,8 @@
       <c r="C96" t="s">
         <v>345</v>
       </c>
-      <c r="D96" s="17" t="s">
-        <v>1532</v>
+      <c r="D96" s="25" t="s">
+        <v>1530</v>
       </c>
       <c r="E96" t="s">
         <v>1278</v>
@@ -9437,8 +9497,8 @@
       <c r="C97" t="s">
         <v>346</v>
       </c>
-      <c r="D97" s="17" t="s">
-        <v>1533</v>
+      <c r="D97" s="25" t="s">
+        <v>1531</v>
       </c>
       <c r="E97" t="s">
         <v>38</v>
@@ -9463,8 +9523,8 @@
       <c r="C98" t="s">
         <v>333</v>
       </c>
-      <c r="D98" s="17" t="s">
-        <v>1491</v>
+      <c r="D98" s="25" t="s">
+        <v>1489</v>
       </c>
       <c r="E98" t="s">
         <v>1251</v>
@@ -9492,8 +9552,8 @@
       <c r="C99" t="s">
         <v>347</v>
       </c>
-      <c r="D99" s="17" t="s">
-        <v>1534</v>
+      <c r="D99" s="25" t="s">
+        <v>1532</v>
       </c>
       <c r="E99" t="s">
         <v>79</v>
@@ -9518,8 +9578,8 @@
       <c r="C100" t="s">
         <v>330</v>
       </c>
-      <c r="D100" s="17" t="s">
-        <v>1487</v>
+      <c r="D100" s="25" t="s">
+        <v>1485</v>
       </c>
       <c r="E100" t="s">
         <v>34</v>
@@ -9544,8 +9604,8 @@
       <c r="C101" t="s">
         <v>348</v>
       </c>
-      <c r="D101" s="17" t="s">
-        <v>1535</v>
+      <c r="D101" s="25" t="s">
+        <v>1533</v>
       </c>
       <c r="E101" t="s">
         <v>81</v>
@@ -9571,7 +9631,7 @@
         <v>349</v>
       </c>
       <c r="D102" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="E102" t="s">
         <v>87</v>
@@ -9596,8 +9656,8 @@
       <c r="C103" t="s">
         <v>350</v>
       </c>
-      <c r="D103" s="17" t="s">
-        <v>1537</v>
+      <c r="D103" s="25" t="s">
+        <v>1535</v>
       </c>
       <c r="E103" t="s">
         <v>84</v>
@@ -9625,8 +9685,8 @@
       <c r="C104" t="s">
         <v>304</v>
       </c>
-      <c r="D104" s="17" t="s">
-        <v>1538</v>
+      <c r="D104" s="25" t="s">
+        <v>1536</v>
       </c>
       <c r="E104" t="s">
         <v>303</v>
@@ -9655,8 +9715,8 @@
       <c r="C105" s="9" t="s">
         <v>1450</v>
       </c>
-      <c r="D105" s="21" t="s">
-        <v>1539</v>
+      <c r="D105" s="26" t="s">
+        <v>1537</v>
       </c>
     </row>
     <row r="106" spans="1:16384" x14ac:dyDescent="0.25">
@@ -9669,8 +9729,8 @@
       <c r="C106" s="9" t="s">
         <v>1456</v>
       </c>
-      <c r="D106" s="21" t="s">
-        <v>1540</v>
+      <c r="D106" s="26" t="s">
+        <v>1538</v>
       </c>
     </row>
     <row r="107" spans="1:16384" x14ac:dyDescent="0.25">
@@ -9683,20 +9743,20 @@
       <c r="C107" s="9" t="s">
         <v>1460</v>
       </c>
-      <c r="D107" s="21" t="s">
-        <v>1541</v>
+      <c r="D107" s="26" t="s">
+        <v>1539</v>
       </c>
     </row>
     <row r="108" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="B108" s="17"/>
       <c r="C108" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="D108" s="17" t="s">
-        <v>1484</v>
+      <c r="D108" s="25" t="s">
+        <v>1482</v>
       </c>
       <c r="E108" s="17"/>
       <c r="F108" s="17"/>
@@ -26093,8 +26153,8 @@
       <c r="C111" t="s">
         <v>338</v>
       </c>
-      <c r="D111" s="17" t="s">
-        <v>1502</v>
+      <c r="D111" s="25" t="s">
+        <v>1500</v>
       </c>
       <c r="E111" t="s">
         <v>53</v>
@@ -26119,8 +26179,8 @@
       <c r="C112" t="s">
         <v>351</v>
       </c>
-      <c r="D112" s="17" t="s">
-        <v>1504</v>
+      <c r="D112" s="25" t="s">
+        <v>1502</v>
       </c>
       <c r="E112" t="s">
         <v>89</v>
@@ -26145,8 +26205,8 @@
       <c r="C113" t="s">
         <v>352</v>
       </c>
-      <c r="D113" s="17" t="s">
-        <v>1542</v>
+      <c r="D113" s="25" t="s">
+        <v>1540</v>
       </c>
       <c r="E113" t="s">
         <v>91</v>
@@ -26171,8 +26231,8 @@
       <c r="C114" t="s">
         <v>353</v>
       </c>
-      <c r="D114" s="17" t="s">
-        <v>1543</v>
+      <c r="D114" s="25" t="s">
+        <v>1541</v>
       </c>
       <c r="E114" t="s">
         <v>93</v>
@@ -26197,8 +26257,8 @@
       <c r="C115" t="s">
         <v>354</v>
       </c>
-      <c r="D115" s="17" t="s">
-        <v>1544</v>
+      <c r="D115" s="25" t="s">
+        <v>1542</v>
       </c>
       <c r="E115" t="s">
         <v>95</v>
@@ -26223,8 +26283,8 @@
       <c r="C116" t="s">
         <v>330</v>
       </c>
-      <c r="D116" s="17" t="s">
-        <v>1487</v>
+      <c r="D116" s="25" t="s">
+        <v>1485</v>
       </c>
       <c r="E116" t="s">
         <v>34</v>
@@ -26249,8 +26309,8 @@
       <c r="C117" t="s">
         <v>348</v>
       </c>
-      <c r="D117" s="17" t="s">
-        <v>1535</v>
+      <c r="D117" s="25" t="s">
+        <v>1533</v>
       </c>
       <c r="E117" t="s">
         <v>81</v>
@@ -26276,8 +26336,8 @@
       <c r="C118" t="s">
         <v>346</v>
       </c>
-      <c r="D118" s="17" t="s">
-        <v>1533</v>
+      <c r="D118" s="25" t="s">
+        <v>1531</v>
       </c>
       <c r="E118" t="s">
         <v>99</v>
@@ -26302,8 +26362,8 @@
       <c r="C119" t="s">
         <v>355</v>
       </c>
-      <c r="D119" s="17" t="s">
-        <v>1545</v>
+      <c r="D119" s="25" t="s">
+        <v>1543</v>
       </c>
       <c r="E119" t="s">
         <v>101</v>
@@ -26328,8 +26388,8 @@
       <c r="C120" t="s">
         <v>338</v>
       </c>
-      <c r="D120" s="17" t="s">
-        <v>1502</v>
+      <c r="D120" s="25" t="s">
+        <v>1500</v>
       </c>
       <c r="E120" t="s">
         <v>53</v>
@@ -26354,8 +26414,8 @@
       <c r="C121" t="s">
         <v>356</v>
       </c>
-      <c r="D121" s="17" t="s">
-        <v>1546</v>
+      <c r="D121" s="25" t="s">
+        <v>1544</v>
       </c>
       <c r="E121" t="s">
         <v>103</v>
@@ -26380,8 +26440,8 @@
       <c r="C122" t="s">
         <v>357</v>
       </c>
-      <c r="D122" s="17" t="s">
-        <v>1547</v>
+      <c r="D122" s="25" t="s">
+        <v>1545</v>
       </c>
       <c r="E122" t="s">
         <v>104</v>
@@ -26406,8 +26466,8 @@
       <c r="C123" t="s">
         <v>358</v>
       </c>
-      <c r="D123" s="17" t="s">
-        <v>1548</v>
+      <c r="D123" s="25" t="s">
+        <v>1546</v>
       </c>
       <c r="E123" t="s">
         <v>105</v>
@@ -26433,8 +26493,8 @@
       <c r="C124" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="D124" s="22" t="s">
-        <v>1549</v>
+      <c r="D124" s="28" t="s">
+        <v>1547</v>
       </c>
       <c r="E124" t="s">
         <v>1279</v>
@@ -26457,8 +26517,8 @@
       <c r="C125" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="D125" s="22" t="s">
-        <v>1550</v>
+      <c r="D125" s="28" t="s">
+        <v>1548</v>
       </c>
       <c r="E125" t="s">
         <v>1280</v>
@@ -26487,8 +26547,8 @@
       <c r="C128" t="s">
         <v>341</v>
       </c>
-      <c r="D128" s="17" t="s">
-        <v>1507</v>
+      <c r="D128" s="25" t="s">
+        <v>1505</v>
       </c>
       <c r="E128" t="s">
         <v>1281</v>
@@ -26513,8 +26573,8 @@
       <c r="C129" t="s">
         <v>314</v>
       </c>
-      <c r="D129" s="17" t="s">
-        <v>1468</v>
+      <c r="D129" s="25" t="s">
+        <v>1467</v>
       </c>
       <c r="E129" t="s">
         <v>1282</v>
@@ -26539,8 +26599,8 @@
       <c r="C130" t="s">
         <v>369</v>
       </c>
-      <c r="D130" s="17" t="s">
-        <v>1551</v>
+      <c r="D130" s="25" t="s">
+        <v>1549</v>
       </c>
       <c r="E130" t="s">
         <v>1283</v>
@@ -26565,8 +26625,8 @@
       <c r="C131" t="s">
         <v>342</v>
       </c>
-      <c r="D131" s="17" t="s">
-        <v>1508</v>
+      <c r="D131" s="25" t="s">
+        <v>1506</v>
       </c>
       <c r="E131" t="s">
         <v>1284</v>
@@ -26591,8 +26651,8 @@
       <c r="C132" t="s">
         <v>370</v>
       </c>
-      <c r="D132" s="17" t="s">
-        <v>1552</v>
+      <c r="D132" s="25" t="s">
+        <v>1550</v>
       </c>
       <c r="E132" t="s">
         <v>1285</v>
@@ -26617,8 +26677,8 @@
       <c r="C133" t="s">
         <v>371</v>
       </c>
-      <c r="D133" s="17" t="s">
-        <v>1553</v>
+      <c r="D133" s="25" t="s">
+        <v>1551</v>
       </c>
       <c r="E133" t="s">
         <v>114</v>
@@ -26644,8 +26704,8 @@
       <c r="C134" t="s">
         <v>372</v>
       </c>
-      <c r="D134" s="17" t="s">
-        <v>1554</v>
+      <c r="D134" s="25" t="s">
+        <v>1552</v>
       </c>
       <c r="E134" t="s">
         <v>1286</v>
@@ -26673,8 +26733,8 @@
       <c r="C135" t="s">
         <v>373</v>
       </c>
-      <c r="D135" s="17" t="s">
-        <v>1555</v>
+      <c r="D135" s="25" t="s">
+        <v>1553</v>
       </c>
       <c r="E135" t="s">
         <v>118</v>
@@ -26699,8 +26759,8 @@
       <c r="C136" t="s">
         <v>294</v>
       </c>
-      <c r="D136" s="17" t="s">
-        <v>1556</v>
+      <c r="D136" s="25" t="s">
+        <v>1554</v>
       </c>
       <c r="E136" t="s">
         <v>295</v>
@@ -26725,8 +26785,8 @@
       <c r="C137" t="s">
         <v>288</v>
       </c>
-      <c r="D137" s="17" t="s">
-        <v>1557</v>
+      <c r="D137" s="25" t="s">
+        <v>1555</v>
       </c>
       <c r="E137" t="s">
         <v>1287</v>
@@ -26751,8 +26811,8 @@
       <c r="C138" t="s">
         <v>374</v>
       </c>
-      <c r="D138" s="17" t="s">
-        <v>1558</v>
+      <c r="D138" s="25" t="s">
+        <v>1556</v>
       </c>
       <c r="E138" t="s">
         <v>1288</v>
@@ -26777,8 +26837,8 @@
       <c r="C139" t="s">
         <v>375</v>
       </c>
-      <c r="D139" s="17" t="s">
-        <v>1559</v>
+      <c r="D139" s="25" t="s">
+        <v>1557</v>
       </c>
       <c r="E139" t="s">
         <v>1289</v>
@@ -26803,8 +26863,8 @@
       <c r="C140" t="s">
         <v>263</v>
       </c>
-      <c r="D140" s="17" t="s">
-        <v>1507</v>
+      <c r="D140" s="25" t="s">
+        <v>1505</v>
       </c>
       <c r="E140" t="s">
         <v>1281</v>
@@ -26836,7 +26896,7 @@
       <c r="C143" t="s">
         <v>376</v>
       </c>
-      <c r="D143" s="17" t="s">
+      <c r="D143" s="25" t="s">
         <v>376</v>
       </c>
       <c r="E143" t="s">
@@ -26872,8 +26932,8 @@
       <c r="C146" t="s">
         <v>130</v>
       </c>
-      <c r="D146" s="17" t="s">
-        <v>1560</v>
+      <c r="D146" s="25" t="s">
+        <v>1558</v>
       </c>
       <c r="E146" t="s">
         <v>1290</v>
@@ -26898,8 +26958,8 @@
       <c r="C147" t="s">
         <v>220</v>
       </c>
-      <c r="D147" s="17" t="s">
-        <v>1561</v>
+      <c r="D147" s="25" t="s">
+        <v>1559</v>
       </c>
       <c r="E147" t="s">
         <v>1291</v>
@@ -26924,8 +26984,8 @@
       <c r="C148" t="s">
         <v>221</v>
       </c>
-      <c r="D148" s="17" t="s">
-        <v>1562</v>
+      <c r="D148" s="25" t="s">
+        <v>1560</v>
       </c>
       <c r="E148" t="s">
         <v>134</v>
@@ -26953,8 +27013,8 @@
       <c r="C149" t="s">
         <v>222</v>
       </c>
-      <c r="D149" s="17" t="s">
-        <v>1563</v>
+      <c r="D149" s="25" t="s">
+        <v>1561</v>
       </c>
       <c r="E149" t="s">
         <v>1292</v>
@@ -26985,8 +27045,8 @@
       <c r="C150" t="s">
         <v>1210</v>
       </c>
-      <c r="D150" s="17" t="s">
-        <v>1564</v>
+      <c r="D150" s="25" t="s">
+        <v>1562</v>
       </c>
       <c r="E150" t="s">
         <v>1293</v>
@@ -27012,8 +27072,8 @@
       <c r="C151" s="3" t="s">
         <v>925</v>
       </c>
-      <c r="D151" s="22" t="s">
-        <v>1615</v>
+      <c r="D151" s="28" t="s">
+        <v>1613</v>
       </c>
       <c r="E151" t="s">
         <v>1325</v>
@@ -27030,8 +27090,8 @@
       <c r="C152" s="3" t="s">
         <v>924</v>
       </c>
-      <c r="D152" s="22" t="s">
-        <v>1614</v>
+      <c r="D152" s="28" t="s">
+        <v>1612</v>
       </c>
       <c r="E152" t="s">
         <v>1324</v>
@@ -27048,8 +27108,8 @@
       <c r="C153" s="3" t="s">
         <v>922</v>
       </c>
-      <c r="D153" s="22" t="s">
-        <v>1612</v>
+      <c r="D153" s="28" t="s">
+        <v>1610</v>
       </c>
       <c r="E153" t="s">
         <v>1322</v>
@@ -27066,8 +27126,8 @@
       <c r="C154" s="3" t="s">
         <v>923</v>
       </c>
-      <c r="D154" s="22" t="s">
-        <v>1613</v>
+      <c r="D154" s="28" t="s">
+        <v>1611</v>
       </c>
       <c r="E154" t="s">
         <v>1323</v>
@@ -27084,8 +27144,8 @@
       <c r="C155" s="3" t="s">
         <v>920</v>
       </c>
-      <c r="D155" s="22" t="s">
-        <v>1611</v>
+      <c r="D155" s="28" t="s">
+        <v>1609</v>
       </c>
       <c r="E155" t="s">
         <v>1320</v>
@@ -27102,8 +27162,8 @@
       <c r="C156" s="3" t="s">
         <v>921</v>
       </c>
-      <c r="D156" s="22" t="s">
-        <v>1473</v>
+      <c r="D156" s="28" t="s">
+        <v>1472</v>
       </c>
       <c r="E156" t="s">
         <v>1321</v>
@@ -27119,8 +27179,8 @@
       <c r="C157" t="s">
         <v>223</v>
       </c>
-      <c r="D157" s="17" t="s">
-        <v>1565</v>
+      <c r="D157" s="25" t="s">
+        <v>1563</v>
       </c>
       <c r="E157" t="s">
         <v>140</v>
@@ -27145,8 +27205,8 @@
       <c r="C158" t="s">
         <v>224</v>
       </c>
-      <c r="D158" s="17" t="s">
-        <v>1566</v>
+      <c r="D158" s="25" t="s">
+        <v>1564</v>
       </c>
       <c r="E158" t="s">
         <v>142</v>
@@ -27171,8 +27231,8 @@
       <c r="C159" t="s">
         <v>225</v>
       </c>
-      <c r="D159" s="17" t="s">
-        <v>1567</v>
+      <c r="D159" s="25" t="s">
+        <v>1565</v>
       </c>
       <c r="E159" t="s">
         <v>144</v>
@@ -27197,8 +27257,8 @@
       <c r="C160" t="s">
         <v>226</v>
       </c>
-      <c r="D160" s="17" t="s">
-        <v>1568</v>
+      <c r="D160" s="25" t="s">
+        <v>1566</v>
       </c>
       <c r="E160" t="s">
         <v>146</v>
@@ -27223,8 +27283,8 @@
       <c r="C161" t="s">
         <v>227</v>
       </c>
-      <c r="D161" s="17" t="s">
-        <v>1569</v>
+      <c r="D161" s="25" t="s">
+        <v>1567</v>
       </c>
       <c r="E161" t="s">
         <v>148</v>
@@ -27249,8 +27309,8 @@
       <c r="C162" t="s">
         <v>230</v>
       </c>
-      <c r="D162" s="17" t="s">
-        <v>1570</v>
+      <c r="D162" s="25" t="s">
+        <v>1568</v>
       </c>
       <c r="E162" t="s">
         <v>1294</v>
@@ -27275,8 +27335,8 @@
       <c r="C163" t="s">
         <v>232</v>
       </c>
-      <c r="D163" s="17" t="s">
-        <v>1571</v>
+      <c r="D163" s="25" t="s">
+        <v>1569</v>
       </c>
       <c r="E163" t="s">
         <v>195</v>
@@ -27301,8 +27361,8 @@
       <c r="C164" t="s">
         <v>233</v>
       </c>
-      <c r="D164" s="17" t="s">
-        <v>1572</v>
+      <c r="D164" s="25" t="s">
+        <v>1570</v>
       </c>
       <c r="E164" t="s">
         <v>1295</v>
@@ -27328,8 +27388,8 @@
       <c r="C165" s="6" t="s">
         <v>573</v>
       </c>
-      <c r="D165" s="22" t="s">
-        <v>1573</v>
+      <c r="D165" s="28" t="s">
+        <v>1571</v>
       </c>
       <c r="F165" s="6" t="s">
         <v>1025</v>
@@ -27348,8 +27408,8 @@
       <c r="C166" t="s">
         <v>234</v>
       </c>
-      <c r="D166" s="17" t="s">
-        <v>1574</v>
+      <c r="D166" s="25" t="s">
+        <v>1572</v>
       </c>
       <c r="E166" t="s">
         <v>1296</v>
@@ -27374,8 +27434,8 @@
       <c r="C167" t="s">
         <v>542</v>
       </c>
-      <c r="D167" s="17" t="s">
-        <v>1576</v>
+      <c r="D167" s="25" t="s">
+        <v>1574</v>
       </c>
       <c r="E167" t="s">
         <v>1297</v>
@@ -27397,8 +27457,8 @@
       <c r="C168" t="s">
         <v>541</v>
       </c>
-      <c r="D168" s="17" t="s">
-        <v>1577</v>
+      <c r="D168" s="25" t="s">
+        <v>1575</v>
       </c>
       <c r="E168" t="s">
         <v>1298</v>
@@ -27423,8 +27483,8 @@
       <c r="C169" t="s">
         <v>538</v>
       </c>
-      <c r="D169" s="17" t="s">
-        <v>1578</v>
+      <c r="D169" s="25" t="s">
+        <v>1576</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>1030</v>
@@ -27443,8 +27503,8 @@
       <c r="C170" t="s">
         <v>235</v>
       </c>
-      <c r="D170" s="17" t="s">
-        <v>1575</v>
+      <c r="D170" s="25" t="s">
+        <v>1573</v>
       </c>
       <c r="E170" t="s">
         <v>154</v>
@@ -27469,8 +27529,8 @@
       <c r="C171" t="s">
         <v>236</v>
       </c>
-      <c r="D171" s="17" t="s">
-        <v>1579</v>
+      <c r="D171" s="25" t="s">
+        <v>1577</v>
       </c>
       <c r="E171" t="s">
         <v>156</v>
@@ -27495,8 +27555,8 @@
       <c r="C172" t="s">
         <v>1179</v>
       </c>
-      <c r="D172" s="17" t="s">
-        <v>1580</v>
+      <c r="D172" s="25" t="s">
+        <v>1578</v>
       </c>
       <c r="E172" t="s">
         <v>158</v>
@@ -27521,8 +27581,8 @@
       <c r="C173" t="s">
         <v>237</v>
       </c>
-      <c r="D173" s="17" t="s">
-        <v>1581</v>
+      <c r="D173" s="25" t="s">
+        <v>1579</v>
       </c>
       <c r="E173" t="s">
         <v>1299</v>
@@ -27547,8 +27607,8 @@
       <c r="C174" t="s">
         <v>238</v>
       </c>
-      <c r="D174" s="17" t="s">
-        <v>1582</v>
+      <c r="D174" s="25" t="s">
+        <v>1580</v>
       </c>
       <c r="E174" t="s">
         <v>1300</v>
@@ -27573,8 +27633,8 @@
       <c r="C175" t="s">
         <v>239</v>
       </c>
-      <c r="D175" s="17" t="s">
-        <v>1583</v>
+      <c r="D175" s="25" t="s">
+        <v>1581</v>
       </c>
       <c r="E175" t="s">
         <v>164</v>
@@ -27599,8 +27659,8 @@
       <c r="C176" t="s">
         <v>240</v>
       </c>
-      <c r="D176" s="17" t="s">
-        <v>1492</v>
+      <c r="D176" s="25" t="s">
+        <v>1490</v>
       </c>
       <c r="E176" t="s">
         <v>166</v>
@@ -27628,7 +27688,9 @@
       <c r="C177" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="D177" s="28"/>
+      <c r="D177" s="29" t="s">
+        <v>1731</v>
+      </c>
       <c r="F177" s="3" t="s">
         <v>1056</v>
       </c>
@@ -27641,7 +27703,9 @@
       <c r="C178" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="D178" s="28"/>
+      <c r="D178" s="29" t="s">
+        <v>1732</v>
+      </c>
       <c r="F178" s="3" t="s">
         <v>1057</v>
       </c>
@@ -27654,7 +27718,9 @@
       <c r="C179" s="3" t="s">
         <v>898</v>
       </c>
-      <c r="D179" s="28"/>
+      <c r="D179" s="29" t="s">
+        <v>1733</v>
+      </c>
       <c r="F179" s="3" t="s">
         <v>1058</v>
       </c>
@@ -27667,8 +27733,8 @@
       <c r="C180" s="3" t="s">
         <v>899</v>
       </c>
-      <c r="D180" s="22" t="s">
-        <v>1606</v>
+      <c r="D180" s="28" t="s">
+        <v>1604</v>
       </c>
       <c r="E180" t="s">
         <v>1315</v>
@@ -27679,13 +27745,15 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="B181" s="3"/>
       <c r="C181" s="3" t="s">
         <v>805</v>
       </c>
-      <c r="D181" s="28"/>
+      <c r="D181" t="s">
+        <v>1669</v>
+      </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
@@ -27695,8 +27763,8 @@
       <c r="C182" s="3" t="s">
         <v>903</v>
       </c>
-      <c r="D182" s="22" t="s">
-        <v>1610</v>
+      <c r="D182" s="28" t="s">
+        <v>1608</v>
       </c>
       <c r="E182" t="s">
         <v>1319</v>
@@ -27707,13 +27775,15 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="B183" s="3"/>
-      <c r="C183" s="30" t="b">
+      <c r="C183" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="D183" s="28"/>
+      <c r="D183" t="s">
+        <v>1734</v>
+      </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
@@ -27723,8 +27793,8 @@
       <c r="C184" s="3" t="s">
         <v>889</v>
       </c>
-      <c r="D184" s="22" t="s">
-        <v>1603</v>
+      <c r="D184" s="28" t="s">
+        <v>1601</v>
       </c>
       <c r="E184" t="s">
         <v>1312</v>
@@ -27741,7 +27811,9 @@
       <c r="C185" s="3" t="s">
         <v>887</v>
       </c>
-      <c r="D185" s="28"/>
+      <c r="D185" t="s">
+        <v>1735</v>
+      </c>
       <c r="E185" t="s">
         <v>1310</v>
       </c>
@@ -27757,8 +27829,8 @@
       <c r="C186" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="D186" s="22" t="s">
-        <v>1605</v>
+      <c r="D186" s="28" t="s">
+        <v>1603</v>
       </c>
       <c r="E186" t="s">
         <v>1314</v>
@@ -27775,8 +27847,8 @@
       <c r="C187" s="9" t="s">
         <v>888</v>
       </c>
-      <c r="D187" s="22" t="s">
-        <v>1602</v>
+      <c r="D187" s="28" t="s">
+        <v>1600</v>
       </c>
       <c r="E187" t="s">
         <v>1311</v>
@@ -27795,7 +27867,7 @@
       <c r="C188" s="3" t="s">
         <v>904</v>
       </c>
-      <c r="D188" s="28"/>
+      <c r="D188" s="30"/>
       <c r="F188" s="3" t="s">
         <v>1050</v>
       </c>
@@ -27808,8 +27880,8 @@
       <c r="C189" s="3" t="s">
         <v>890</v>
       </c>
-      <c r="D189" s="22" t="s">
-        <v>1604</v>
+      <c r="D189" s="28" t="s">
+        <v>1602</v>
       </c>
       <c r="E189" t="s">
         <v>1313</v>
@@ -27826,8 +27898,8 @@
       <c r="C190" s="3" t="s">
         <v>900</v>
       </c>
-      <c r="D190" s="22" t="s">
-        <v>1607</v>
+      <c r="D190" s="28" t="s">
+        <v>1605</v>
       </c>
       <c r="E190" t="s">
         <v>1316</v>
@@ -27844,8 +27916,8 @@
       <c r="C191" s="3" t="s">
         <v>901</v>
       </c>
-      <c r="D191" s="22" t="s">
-        <v>1608</v>
+      <c r="D191" s="28" t="s">
+        <v>1606</v>
       </c>
       <c r="E191" t="s">
         <v>1317</v>
@@ -27862,8 +27934,8 @@
       <c r="C192" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="D192" s="22" t="s">
-        <v>1609</v>
+      <c r="D192" s="28" t="s">
+        <v>1607</v>
       </c>
       <c r="E192" t="s">
         <v>1318</v>
@@ -27874,13 +27946,13 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="B193" s="3"/>
-      <c r="C193" s="31" t="b">
+      <c r="C193" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="D193" s="22"/>
+      <c r="D193" s="28"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
@@ -27890,8 +27962,8 @@
       <c r="C194" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="D194" s="22" t="s">
-        <v>1530</v>
+      <c r="D194" s="28" t="s">
+        <v>1528</v>
       </c>
       <c r="E194" t="s">
         <v>1276</v>
@@ -27907,8 +27979,8 @@
       <c r="C195" t="s">
         <v>241</v>
       </c>
-      <c r="D195" s="17" t="s">
-        <v>1584</v>
+      <c r="D195" s="25" t="s">
+        <v>1582</v>
       </c>
       <c r="E195" t="s">
         <v>1301</v>
@@ -27933,8 +28005,8 @@
       <c r="C196" t="s">
         <v>242</v>
       </c>
-      <c r="D196" s="17" t="s">
-        <v>1585</v>
+      <c r="D196" s="25" t="s">
+        <v>1583</v>
       </c>
       <c r="E196" t="s">
         <v>1302</v>
@@ -27959,8 +28031,8 @@
       <c r="C197" t="s">
         <v>245</v>
       </c>
-      <c r="D197" s="17" t="s">
-        <v>1539</v>
+      <c r="D197" s="25" t="s">
+        <v>1537</v>
       </c>
       <c r="E197" t="s">
         <v>244</v>
@@ -27985,8 +28057,8 @@
       <c r="C198" t="s">
         <v>248</v>
       </c>
-      <c r="D198" s="17" t="s">
-        <v>1586</v>
+      <c r="D198" s="25" t="s">
+        <v>1584</v>
       </c>
       <c r="E198" t="s">
         <v>247</v>
@@ -28011,8 +28083,8 @@
       <c r="C199" t="s">
         <v>249</v>
       </c>
-      <c r="D199" s="17" t="s">
-        <v>1587</v>
+      <c r="D199" s="25" t="s">
+        <v>1585</v>
       </c>
       <c r="E199" t="s">
         <v>172</v>
@@ -28038,8 +28110,8 @@
       <c r="C200" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="D200" s="22" t="s">
-        <v>1588</v>
+      <c r="D200" s="28" t="s">
+        <v>1586</v>
       </c>
       <c r="F200" s="6" t="s">
         <v>1041</v>
@@ -28058,8 +28130,8 @@
       <c r="C201" t="s">
         <v>250</v>
       </c>
-      <c r="D201" s="17" t="s">
-        <v>1589</v>
+      <c r="D201" s="25" t="s">
+        <v>1587</v>
       </c>
       <c r="E201" t="s">
         <v>174</v>
@@ -28087,8 +28159,8 @@
       <c r="C202" t="s">
         <v>1211</v>
       </c>
-      <c r="D202" s="23" t="s">
-        <v>1590</v>
+      <c r="D202" s="25" t="s">
+        <v>1588</v>
       </c>
       <c r="E202" t="s">
         <v>176</v>
@@ -28113,8 +28185,8 @@
       <c r="C203" t="s">
         <v>251</v>
       </c>
-      <c r="D203" s="17" t="s">
-        <v>1591</v>
+      <c r="D203" s="25" t="s">
+        <v>1589</v>
       </c>
       <c r="E203" t="s">
         <v>178</v>
@@ -28142,8 +28214,8 @@
       <c r="C204" t="s">
         <v>1212</v>
       </c>
-      <c r="D204" s="17" t="s">
-        <v>1592</v>
+      <c r="D204" s="25" t="s">
+        <v>1590</v>
       </c>
       <c r="E204" t="s">
         <v>180</v>
@@ -28171,8 +28243,8 @@
       <c r="C205" t="s">
         <v>1213</v>
       </c>
-      <c r="D205" s="17" t="s">
-        <v>1593</v>
+      <c r="D205" s="25" t="s">
+        <v>1591</v>
       </c>
       <c r="E205" t="s">
         <v>1303</v>
@@ -28200,8 +28272,8 @@
       <c r="C206" t="s">
         <v>1214</v>
       </c>
-      <c r="D206" s="17" t="s">
-        <v>1594</v>
+      <c r="D206" s="25" t="s">
+        <v>1592</v>
       </c>
       <c r="E206" t="s">
         <v>1304</v>
@@ -28226,8 +28298,8 @@
       <c r="C207" t="s">
         <v>252</v>
       </c>
-      <c r="D207" s="17" t="s">
-        <v>1595</v>
+      <c r="D207" s="25" t="s">
+        <v>1593</v>
       </c>
       <c r="E207" t="s">
         <v>1305</v>
@@ -28252,8 +28324,8 @@
       <c r="C208" t="s">
         <v>544</v>
       </c>
-      <c r="D208" s="17" t="s">
-        <v>1596</v>
+      <c r="D208" s="25" t="s">
+        <v>1594</v>
       </c>
       <c r="E208" t="s">
         <v>188</v>
@@ -28278,8 +28350,8 @@
       <c r="C209" t="s">
         <v>253</v>
       </c>
-      <c r="D209" s="17" t="s">
-        <v>1597</v>
+      <c r="D209" s="25" t="s">
+        <v>1595</v>
       </c>
       <c r="E209" t="s">
         <v>190</v>
@@ -28304,8 +28376,8 @@
       <c r="C210" t="s">
         <v>254</v>
       </c>
-      <c r="D210" s="17" t="s">
-        <v>1598</v>
+      <c r="D210" s="25" t="s">
+        <v>1596</v>
       </c>
       <c r="E210" t="s">
         <v>1306</v>
@@ -28330,8 +28402,8 @@
       <c r="C211" t="s">
         <v>193</v>
       </c>
-      <c r="D211" s="17" t="s">
-        <v>1599</v>
+      <c r="D211" s="25" t="s">
+        <v>1597</v>
       </c>
       <c r="E211" t="s">
         <v>1307</v>
@@ -28356,7 +28428,7 @@
       <c r="C212" t="s">
         <v>255</v>
       </c>
-      <c r="D212" s="17" t="s">
+      <c r="D212" s="25" t="s">
         <v>255</v>
       </c>
       <c r="E212" t="s">
@@ -28382,8 +28454,8 @@
       <c r="C213" t="s">
         <v>820</v>
       </c>
-      <c r="D213" s="17" t="s">
-        <v>1600</v>
+      <c r="D213" s="25" t="s">
+        <v>1598</v>
       </c>
       <c r="E213" t="s">
         <v>199</v>
@@ -28408,8 +28480,8 @@
       <c r="C214" t="s">
         <v>256</v>
       </c>
-      <c r="D214" s="17" t="s">
-        <v>1601</v>
+      <c r="D214" s="25" t="s">
+        <v>1599</v>
       </c>
       <c r="E214" t="s">
         <v>1309</v>
@@ -28442,8 +28514,8 @@
       <c r="C217" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D217" s="22" t="s">
-        <v>1616</v>
+      <c r="D217" s="28" t="s">
+        <v>1614</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>1326</v>
@@ -28466,8 +28538,8 @@
       <c r="C218" t="s">
         <v>523</v>
       </c>
-      <c r="D218" s="17" t="s">
-        <v>1617</v>
+      <c r="D218" s="25" t="s">
+        <v>1615</v>
       </c>
       <c r="E218" t="s">
         <v>1327</v>
@@ -28481,13 +28553,15 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s">
-        <v>1697</v>
-      </c>
-      <c r="D219" s="28"/>
+        <v>1695</v>
+      </c>
+      <c r="D219" t="s">
+        <v>1736</v>
+      </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
@@ -28496,8 +28570,8 @@
       <c r="C220" t="s">
         <v>245</v>
       </c>
-      <c r="D220" s="17" t="s">
-        <v>1539</v>
+      <c r="D220" s="25" t="s">
+        <v>1537</v>
       </c>
       <c r="E220" t="s">
         <v>244</v>
@@ -28525,8 +28599,8 @@
       <c r="C221" t="s">
         <v>248</v>
       </c>
-      <c r="D221" s="17" t="s">
-        <v>1586</v>
+      <c r="D221" s="25" t="s">
+        <v>1584</v>
       </c>
       <c r="E221" t="s">
         <v>247</v>
@@ -28554,8 +28628,8 @@
       <c r="C222" t="s">
         <v>522</v>
       </c>
-      <c r="D222" s="17" t="s">
-        <v>1618</v>
+      <c r="D222" s="25" t="s">
+        <v>1616</v>
       </c>
       <c r="E222" t="s">
         <v>1328</v>
@@ -28577,8 +28651,8 @@
       <c r="C223" t="s">
         <v>261</v>
       </c>
-      <c r="D223" s="17" t="s">
-        <v>1619</v>
+      <c r="D223" s="25" t="s">
+        <v>1617</v>
       </c>
       <c r="E223" t="s">
         <v>1329</v>
@@ -28606,8 +28680,8 @@
       <c r="C224" t="s">
         <v>263</v>
       </c>
-      <c r="D224" s="17" t="s">
-        <v>1620</v>
+      <c r="D224" s="25" t="s">
+        <v>1618</v>
       </c>
       <c r="E224" t="s">
         <v>1330</v>
@@ -28635,7 +28709,7 @@
       <c r="C225" t="s">
         <v>266</v>
       </c>
-      <c r="D225" s="17" t="s">
+      <c r="D225" s="25" t="s">
         <v>266</v>
       </c>
       <c r="E225" t="s">
@@ -28665,8 +28739,8 @@
       <c r="C226" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="D226" s="22" t="s">
-        <v>1635</v>
+      <c r="D226" s="28" t="s">
+        <v>1633</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>1335</v>
@@ -28689,8 +28763,8 @@
       <c r="C227" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="D227" s="22" t="s">
-        <v>1621</v>
+      <c r="D227" s="28" t="s">
+        <v>1619</v>
       </c>
       <c r="E227" t="s">
         <v>1331</v>
@@ -28709,8 +28783,8 @@
       <c r="C228" t="s">
         <v>269</v>
       </c>
-      <c r="D228" s="17" t="s">
-        <v>1622</v>
+      <c r="D228" s="25" t="s">
+        <v>1620</v>
       </c>
       <c r="E228" t="s">
         <v>268</v>
@@ -28738,8 +28812,8 @@
       <c r="C229" t="s">
         <v>272</v>
       </c>
-      <c r="D229" s="17" t="s">
-        <v>1623</v>
+      <c r="D229" s="25" t="s">
+        <v>1621</v>
       </c>
       <c r="E229" t="s">
         <v>1332</v>
@@ -28767,8 +28841,8 @@
       <c r="C230" t="s">
         <v>269</v>
       </c>
-      <c r="D230" s="17" t="s">
-        <v>1622</v>
+      <c r="D230" s="25" t="s">
+        <v>1620</v>
       </c>
       <c r="E230" t="s">
         <v>268</v>
@@ -28796,8 +28870,8 @@
       <c r="C231" t="s">
         <v>276</v>
       </c>
-      <c r="D231" s="17" t="s">
-        <v>1624</v>
+      <c r="D231" s="25" t="s">
+        <v>1622</v>
       </c>
       <c r="E231" t="s">
         <v>275</v>
@@ -28825,8 +28899,8 @@
       <c r="C232" t="s">
         <v>278</v>
       </c>
-      <c r="D232" s="17" t="s">
-        <v>1625</v>
+      <c r="D232" s="25" t="s">
+        <v>1623</v>
       </c>
       <c r="E232" t="s">
         <v>1333</v>
@@ -28854,8 +28928,8 @@
       <c r="C233" t="s">
         <v>281</v>
       </c>
-      <c r="D233" s="17" t="s">
-        <v>1626</v>
+      <c r="D233" s="25" t="s">
+        <v>1624</v>
       </c>
       <c r="E233" t="s">
         <v>1334</v>
@@ -28883,8 +28957,8 @@
       <c r="C234" t="s">
         <v>284</v>
       </c>
-      <c r="D234" s="17" t="s">
-        <v>1627</v>
+      <c r="D234" s="25" t="s">
+        <v>1625</v>
       </c>
       <c r="E234" t="s">
         <v>283</v>
@@ -28912,8 +28986,8 @@
       <c r="C235" t="s">
         <v>287</v>
       </c>
-      <c r="D235" s="17" t="s">
-        <v>1628</v>
+      <c r="D235" s="25" t="s">
+        <v>1626</v>
       </c>
       <c r="E235" t="s">
         <v>286</v>
@@ -28941,8 +29015,8 @@
       <c r="C236" t="s">
         <v>290</v>
       </c>
-      <c r="D236" s="17" t="s">
-        <v>1629</v>
+      <c r="D236" s="25" t="s">
+        <v>1627</v>
       </c>
       <c r="E236" t="s">
         <v>289</v>
@@ -28970,8 +29044,8 @@
       <c r="C237" t="s">
         <v>293</v>
       </c>
-      <c r="D237" s="17" t="s">
-        <v>1630</v>
+      <c r="D237" s="25" t="s">
+        <v>1628</v>
       </c>
       <c r="E237" t="s">
         <v>292</v>
@@ -29000,8 +29074,8 @@
       <c r="C238" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="D238" s="22" t="s">
-        <v>1488</v>
+      <c r="D238" s="28" t="s">
+        <v>1486</v>
       </c>
       <c r="E238" s="3" t="s">
         <v>1249</v>
@@ -29024,8 +29098,8 @@
       <c r="C239" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="D239" s="22" t="s">
-        <v>1489</v>
+      <c r="D239" s="28" t="s">
+        <v>1487</v>
       </c>
       <c r="E239" s="3" t="s">
         <v>1250</v>
@@ -29047,8 +29121,8 @@
       <c r="C240" t="s">
         <v>294</v>
       </c>
-      <c r="D240" s="17" t="s">
-        <v>1631</v>
+      <c r="D240" s="25" t="s">
+        <v>1629</v>
       </c>
       <c r="E240" t="s">
         <v>295</v>
@@ -29076,8 +29150,8 @@
       <c r="C241" t="s">
         <v>298</v>
       </c>
-      <c r="D241" s="17" t="s">
-        <v>1632</v>
+      <c r="D241" s="25" t="s">
+        <v>1630</v>
       </c>
       <c r="E241" t="s">
         <v>297</v>
@@ -29105,8 +29179,8 @@
       <c r="C242" t="s">
         <v>278</v>
       </c>
-      <c r="D242" s="17" t="s">
-        <v>1625</v>
+      <c r="D242" s="25" t="s">
+        <v>1623</v>
       </c>
       <c r="E242" t="s">
         <v>277</v>
@@ -29134,8 +29208,8 @@
       <c r="C243" t="s">
         <v>301</v>
       </c>
-      <c r="D243" s="17" t="s">
-        <v>1633</v>
+      <c r="D243" s="25" t="s">
+        <v>1631</v>
       </c>
       <c r="E243" t="s">
         <v>300</v>
@@ -29163,8 +29237,8 @@
       <c r="C244" t="s">
         <v>304</v>
       </c>
-      <c r="D244" s="17" t="s">
-        <v>1538</v>
+      <c r="D244" s="25" t="s">
+        <v>1536</v>
       </c>
       <c r="E244" t="s">
         <v>303</v>
@@ -29192,8 +29266,8 @@
       <c r="C245" t="s">
         <v>307</v>
       </c>
-      <c r="D245" s="17" t="s">
-        <v>1634</v>
+      <c r="D245" s="25" t="s">
+        <v>1632</v>
       </c>
       <c r="E245" t="s">
         <v>306</v>
@@ -29228,8 +29302,8 @@
       <c r="C248" t="s">
         <v>334</v>
       </c>
-      <c r="D248" s="17" t="s">
-        <v>1493</v>
+      <c r="D248" s="25" t="s">
+        <v>1491</v>
       </c>
       <c r="E248" t="s">
         <v>44</v>
@@ -29257,7 +29331,9 @@
       <c r="C249" t="s">
         <v>377</v>
       </c>
-      <c r="D249" s="28"/>
+      <c r="D249" t="s">
+        <v>1737</v>
+      </c>
       <c r="E249" t="s">
         <v>1336</v>
       </c>
@@ -29291,8 +29367,8 @@
       <c r="C252" t="s">
         <v>344</v>
       </c>
-      <c r="D252" s="17" t="s">
-        <v>1531</v>
+      <c r="D252" s="25" t="s">
+        <v>1529</v>
       </c>
       <c r="E252" t="s">
         <v>1337</v>
@@ -29317,8 +29393,8 @@
       <c r="C253" t="s">
         <v>330</v>
       </c>
-      <c r="D253" s="17" t="s">
-        <v>1487</v>
+      <c r="D253" s="25" t="s">
+        <v>1485</v>
       </c>
       <c r="E253" t="s">
         <v>34</v>
@@ -29343,8 +29419,8 @@
       <c r="C254" t="s">
         <v>348</v>
       </c>
-      <c r="D254" s="17" t="s">
-        <v>1535</v>
+      <c r="D254" s="25" t="s">
+        <v>1533</v>
       </c>
       <c r="E254" t="s">
         <v>81</v>
@@ -29369,8 +29445,8 @@
       <c r="C255" t="s">
         <v>346</v>
       </c>
-      <c r="D255" s="17" t="s">
-        <v>1533</v>
+      <c r="D255" s="25" t="s">
+        <v>1531</v>
       </c>
       <c r="E255" t="s">
         <v>38</v>
@@ -29395,8 +29471,8 @@
       <c r="C256" t="s">
         <v>333</v>
       </c>
-      <c r="D256" s="17" t="s">
-        <v>1491</v>
+      <c r="D256" s="25" t="s">
+        <v>1489</v>
       </c>
       <c r="E256" t="s">
         <v>40</v>
@@ -29421,8 +29497,8 @@
       <c r="C257" t="s">
         <v>533</v>
       </c>
-      <c r="D257" s="17" t="s">
-        <v>1636</v>
+      <c r="D257" s="25" t="s">
+        <v>1634</v>
       </c>
       <c r="E257" t="s">
         <v>1338</v>
@@ -29446,7 +29522,7 @@
       </c>
       <c r="B259" s="10"/>
       <c r="C259" s="3"/>
-      <c r="D259" s="22"/>
+      <c r="D259" s="28"/>
       <c r="G259" s="3"/>
     </row>
     <row r="260" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -29457,8 +29533,8 @@
       <c r="C260" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="D260" s="22" t="s">
-        <v>1637</v>
+      <c r="D260" s="28" t="s">
+        <v>1635</v>
       </c>
       <c r="F260" s="3" t="s">
         <v>1091</v>
@@ -29471,7 +29547,7 @@
       <c r="A261" s="8"/>
       <c r="B261" s="8"/>
       <c r="C261" s="8"/>
-      <c r="D261" s="24"/>
+      <c r="D261" s="31"/>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="10" t="s">
@@ -29479,7 +29555,7 @@
       </c>
       <c r="B262" s="10"/>
       <c r="C262" s="3"/>
-      <c r="D262" s="22"/>
+      <c r="D262" s="28"/>
       <c r="G262" s="3"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
@@ -29490,8 +29566,8 @@
       <c r="C263" s="3" t="s">
         <v>872</v>
       </c>
-      <c r="D263" s="22" t="s">
-        <v>1638</v>
+      <c r="D263" s="28" t="s">
+        <v>1636</v>
       </c>
       <c r="E263" t="s">
         <v>1339</v>
@@ -29511,8 +29587,8 @@
       <c r="C264" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D264" s="22" t="s">
-        <v>1493</v>
+      <c r="D264" s="28" t="s">
+        <v>1491</v>
       </c>
       <c r="E264" t="s">
         <v>1350</v>
@@ -29532,8 +29608,8 @@
       <c r="C265" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="D265" s="22" t="s">
-        <v>1640</v>
+      <c r="D265" s="28" t="s">
+        <v>1638</v>
       </c>
       <c r="E265" t="s">
         <v>1341</v>
@@ -29553,8 +29629,8 @@
       <c r="C266" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="D266" s="22" t="s">
-        <v>1641</v>
+      <c r="D266" s="28" t="s">
+        <v>1639</v>
       </c>
       <c r="E266" t="s">
         <v>1342</v>
@@ -29571,8 +29647,8 @@
       <c r="C267" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D267" s="22" t="s">
-        <v>1557</v>
+      <c r="D267" s="28" t="s">
+        <v>1555</v>
       </c>
       <c r="E267" t="s">
         <v>1287</v>
@@ -29592,8 +29668,8 @@
       <c r="C268" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D268" s="22" t="s">
-        <v>1557</v>
+      <c r="D268" s="28" t="s">
+        <v>1555</v>
       </c>
       <c r="E268" t="s">
         <v>1287</v>
@@ -29613,8 +29689,8 @@
       <c r="C269" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="D269" s="22" t="s">
-        <v>1639</v>
+      <c r="D269" s="28" t="s">
+        <v>1637</v>
       </c>
       <c r="E269" t="s">
         <v>1340</v>
@@ -29636,8 +29712,8 @@
       <c r="C270" s="3" t="s">
         <v>1217</v>
       </c>
-      <c r="D270" s="22" t="s">
-        <v>1648</v>
+      <c r="D270" s="28" t="s">
+        <v>1646</v>
       </c>
       <c r="E270" s="3" t="s">
         <v>1349</v>
@@ -29654,8 +29730,8 @@
       <c r="C271" s="3" t="s">
         <v>1235</v>
       </c>
-      <c r="D271" s="22" t="s">
-        <v>1646</v>
+      <c r="D271" s="28" t="s">
+        <v>1644</v>
       </c>
       <c r="E271" t="s">
         <v>1347</v>
@@ -29672,8 +29748,8 @@
       <c r="C272" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="D272" s="22" t="s">
-        <v>1646</v>
+      <c r="D272" s="28" t="s">
+        <v>1644</v>
       </c>
       <c r="E272" t="s">
         <v>1347</v>
@@ -29690,8 +29766,8 @@
       <c r="C273" s="3" t="s">
         <v>934</v>
       </c>
-      <c r="D273" s="22" t="s">
-        <v>1642</v>
+      <c r="D273" s="28" t="s">
+        <v>1640</v>
       </c>
       <c r="E273" t="s">
         <v>1343</v>
@@ -29708,8 +29784,8 @@
       <c r="C274" s="3" t="s">
         <v>935</v>
       </c>
-      <c r="D274" s="22" t="s">
-        <v>1643</v>
+      <c r="D274" s="28" t="s">
+        <v>1641</v>
       </c>
       <c r="E274" t="s">
         <v>1344</v>
@@ -29726,8 +29802,8 @@
       <c r="C275" s="3" t="s">
         <v>937</v>
       </c>
-      <c r="D275" s="22" t="s">
-        <v>1644</v>
+      <c r="D275" s="28" t="s">
+        <v>1642</v>
       </c>
       <c r="E275" t="s">
         <v>1345</v>
@@ -29744,8 +29820,8 @@
       <c r="C276" s="3" t="s">
         <v>939</v>
       </c>
-      <c r="D276" s="22" t="s">
-        <v>1645</v>
+      <c r="D276" s="28" t="s">
+        <v>1643</v>
       </c>
       <c r="E276" t="s">
         <v>1346</v>
@@ -29762,8 +29838,8 @@
       <c r="C277" s="3" t="s">
         <v>942</v>
       </c>
-      <c r="D277" s="22" t="s">
-        <v>1647</v>
+      <c r="D277" s="28" t="s">
+        <v>1645</v>
       </c>
       <c r="E277" t="s">
         <v>1348</v>
@@ -29776,7 +29852,7 @@
       <c r="A278" s="8"/>
       <c r="B278" s="8"/>
       <c r="C278" s="8"/>
-      <c r="D278" s="24"/>
+      <c r="D278" s="31"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="10" t="s">
@@ -29784,7 +29860,7 @@
       </c>
       <c r="B279" s="10"/>
       <c r="C279" s="3"/>
-      <c r="D279" s="22"/>
+      <c r="D279" s="28"/>
       <c r="G279" s="3"/>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -29795,8 +29871,8 @@
       <c r="C280" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="D280" s="22" t="s">
-        <v>1649</v>
+      <c r="D280" s="28" t="s">
+        <v>1647</v>
       </c>
       <c r="E280" t="s">
         <v>1351</v>
@@ -29816,8 +29892,8 @@
       <c r="C281" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D281" s="21" t="s">
-        <v>1477</v>
+      <c r="D281" s="26" t="s">
+        <v>1476</v>
       </c>
       <c r="E281" t="s">
         <v>15</v>
@@ -29832,8 +29908,8 @@
       <c r="C282" s="9" t="s">
         <v>773</v>
       </c>
-      <c r="D282" s="21" t="s">
-        <v>1651</v>
+      <c r="D282" s="26" t="s">
+        <v>1649</v>
       </c>
       <c r="E282" t="s">
         <v>1362</v>
@@ -29848,8 +29924,8 @@
       <c r="C283" s="9" t="s">
         <v>772</v>
       </c>
-      <c r="D283" s="21" t="s">
-        <v>1652</v>
+      <c r="D283" s="26" t="s">
+        <v>1650</v>
       </c>
       <c r="E283" t="s">
         <v>1361</v>
@@ -29864,8 +29940,8 @@
       <c r="C284" s="9" t="s">
         <v>878</v>
       </c>
-      <c r="D284" s="21" t="s">
-        <v>1650</v>
+      <c r="D284" s="26" t="s">
+        <v>1648</v>
       </c>
       <c r="E284" t="s">
         <v>1352</v>
@@ -29885,7 +29961,7 @@
       <c r="C285" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="D285" s="21" t="s">
+      <c r="D285" s="26" t="s">
         <v>1464</v>
       </c>
       <c r="E285" t="s">
@@ -29901,8 +29977,8 @@
       <c r="C286" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="D286" s="22" t="s">
-        <v>1639</v>
+      <c r="D286" s="28" t="s">
+        <v>1637</v>
       </c>
       <c r="E286" t="s">
         <v>1365</v>
@@ -29922,8 +29998,8 @@
       <c r="C287" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="D287" s="22" t="s">
-        <v>1526</v>
+      <c r="D287" s="28" t="s">
+        <v>1524</v>
       </c>
       <c r="E287" t="s">
         <v>1265</v>
@@ -29943,8 +30019,8 @@
       <c r="C288" s="3" t="s">
         <v>771</v>
       </c>
-      <c r="D288" s="22" t="s">
-        <v>1660</v>
+      <c r="D288" s="28" t="s">
+        <v>1658</v>
       </c>
       <c r="E288" t="s">
         <v>1360</v>
@@ -29964,8 +30040,8 @@
       <c r="C289" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="D289" s="22" t="s">
-        <v>1526</v>
+      <c r="D289" s="28" t="s">
+        <v>1524</v>
       </c>
       <c r="E289" t="s">
         <v>1265</v>
@@ -29985,8 +30061,8 @@
       <c r="C290" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="D290" s="22" t="s">
-        <v>1655</v>
+      <c r="D290" s="28" t="s">
+        <v>1653</v>
       </c>
       <c r="E290" t="s">
         <v>1355</v>
@@ -30006,8 +30082,8 @@
       <c r="C291" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D291" s="22" t="s">
-        <v>1533</v>
+      <c r="D291" s="28" t="s">
+        <v>1531</v>
       </c>
       <c r="E291" t="s">
         <v>38</v>
@@ -30022,8 +30098,8 @@
       <c r="C292" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D292" s="22" t="s">
-        <v>1654</v>
+      <c r="D292" s="28" t="s">
+        <v>1652</v>
       </c>
       <c r="E292" t="s">
         <v>1354</v>
@@ -30043,8 +30119,8 @@
       <c r="C293" s="3" t="s">
         <v>1405</v>
       </c>
-      <c r="D293" s="22" t="s">
-        <v>1656</v>
+      <c r="D293" s="28" t="s">
+        <v>1654</v>
       </c>
       <c r="E293" t="s">
         <v>1356</v>
@@ -30064,8 +30140,8 @@
       <c r="C294" s="3" t="s">
         <v>1406</v>
       </c>
-      <c r="D294" s="22" t="s">
-        <v>1657</v>
+      <c r="D294" s="28" t="s">
+        <v>1655</v>
       </c>
       <c r="E294" t="s">
         <v>1357</v>
@@ -30085,8 +30161,8 @@
       <c r="C295" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="D295" s="22" t="s">
-        <v>1659</v>
+      <c r="D295" s="28" t="s">
+        <v>1657</v>
       </c>
       <c r="E295" t="s">
         <v>1359</v>
@@ -30106,8 +30182,8 @@
       <c r="C296" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="D296" s="22" t="s">
-        <v>1662</v>
+      <c r="D296" s="28" t="s">
+        <v>1660</v>
       </c>
       <c r="E296" t="s">
         <v>1364</v>
@@ -30121,13 +30197,15 @@
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="B297" s="3"/>
       <c r="C297" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="D297" s="28"/>
+        <v>1697</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1738</v>
+      </c>
       <c r="G297" s="3"/>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
@@ -30138,8 +30216,8 @@
       <c r="C298" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D298" s="22" t="s">
-        <v>1533</v>
+      <c r="D298" s="28" t="s">
+        <v>1739</v>
       </c>
       <c r="E298" t="s">
         <v>38</v>
@@ -30159,8 +30237,8 @@
       <c r="C299" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D299" s="22" t="s">
-        <v>1663</v>
+      <c r="D299" s="28" t="s">
+        <v>1661</v>
       </c>
       <c r="G299" s="3"/>
     </row>
@@ -30172,8 +30250,8 @@
       <c r="C300" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="D300" s="22" t="s">
-        <v>1653</v>
+      <c r="D300" s="28" t="s">
+        <v>1651</v>
       </c>
       <c r="E300" t="s">
         <v>1353</v>
@@ -30193,8 +30271,8 @@
       <c r="C301" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="D301" s="22" t="s">
-        <v>1658</v>
+      <c r="D301" s="28" t="s">
+        <v>1656</v>
       </c>
       <c r="E301" t="s">
         <v>1358</v>
@@ -30214,8 +30292,8 @@
       <c r="C302" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="D302" s="22" t="s">
-        <v>1661</v>
+      <c r="D302" s="28" t="s">
+        <v>1659</v>
       </c>
       <c r="E302" t="s">
         <v>1363</v>
@@ -30235,8 +30313,8 @@
       <c r="C303" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D303" s="22" t="s">
-        <v>1477</v>
+      <c r="D303" s="28" t="s">
+        <v>1476</v>
       </c>
       <c r="E303" t="s">
         <v>15</v>
@@ -30256,8 +30334,8 @@
       <c r="C304" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="D304" s="22" t="s">
-        <v>1651</v>
+      <c r="D304" s="28" t="s">
+        <v>1649</v>
       </c>
       <c r="E304" t="s">
         <v>1362</v>
@@ -30277,8 +30355,8 @@
       <c r="C305" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="D305" s="22" t="s">
-        <v>1652</v>
+      <c r="D305" s="28" t="s">
+        <v>1650</v>
       </c>
       <c r="E305" t="s">
         <v>1361</v>
@@ -30294,7 +30372,7 @@
       <c r="A306" s="8"/>
       <c r="B306" s="8"/>
       <c r="C306" s="8"/>
-      <c r="D306" s="24"/>
+      <c r="D306" s="31"/>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="10" t="s">
@@ -30302,7 +30380,7 @@
       </c>
       <c r="B307" s="10"/>
       <c r="C307" s="3"/>
-      <c r="D307" s="22"/>
+      <c r="D307" s="28"/>
       <c r="G307" s="3"/>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
@@ -30313,8 +30391,8 @@
       <c r="C308" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="D308" s="22" t="s">
-        <v>1664</v>
+      <c r="D308" s="28" t="s">
+        <v>1662</v>
       </c>
       <c r="E308" t="s">
         <v>1366</v>
@@ -30334,8 +30412,8 @@
       <c r="C309" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D309" s="22" t="s">
-        <v>1477</v>
+      <c r="D309" s="28" t="s">
+        <v>1476</v>
       </c>
       <c r="E309" t="s">
         <v>15</v>
@@ -30355,8 +30433,8 @@
       <c r="C310" s="3" t="s">
         <v>785</v>
       </c>
-      <c r="D310" s="22" t="s">
-        <v>1606</v>
+      <c r="D310" s="28" t="s">
+        <v>1604</v>
       </c>
       <c r="E310" t="s">
         <v>1257</v>
@@ -30376,8 +30454,8 @@
       <c r="C311" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="D311" s="22" t="s">
-        <v>1671</v>
+      <c r="D311" s="28" t="s">
+        <v>1669</v>
       </c>
       <c r="E311" t="s">
         <v>1372</v>
@@ -30397,8 +30475,8 @@
       <c r="C312" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="D312" s="22" t="s">
-        <v>1670</v>
+      <c r="D312" s="28" t="s">
+        <v>1668</v>
       </c>
       <c r="E312" t="s">
         <v>1371</v>
@@ -30418,8 +30496,8 @@
       <c r="C313" s="3" t="s">
         <v>781</v>
       </c>
-      <c r="D313" s="22" t="s">
-        <v>1667</v>
+      <c r="D313" s="28" t="s">
+        <v>1665</v>
       </c>
       <c r="E313" t="s">
         <v>1368</v>
@@ -30439,8 +30517,8 @@
       <c r="C314" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D314" s="22" t="s">
-        <v>1533</v>
+      <c r="D314" s="28" t="s">
+        <v>1531</v>
       </c>
       <c r="E314" t="s">
         <v>38</v>
@@ -30460,8 +30538,8 @@
       <c r="C315" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D315" s="22" t="s">
-        <v>1672</v>
+      <c r="D315" s="28" t="s">
+        <v>1670</v>
       </c>
       <c r="E315" t="s">
         <v>166</v>
@@ -30481,8 +30559,8 @@
       <c r="C316" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="D316" s="22" t="s">
-        <v>1666</v>
+      <c r="D316" s="28" t="s">
+        <v>1664</v>
       </c>
       <c r="E316" t="s">
         <v>1367</v>
@@ -30502,8 +30580,8 @@
       <c r="C317" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="D317" s="22" t="s">
-        <v>1668</v>
+      <c r="D317" s="28" t="s">
+        <v>1666</v>
       </c>
       <c r="E317" t="s">
         <v>1369</v>
@@ -30523,8 +30601,8 @@
       <c r="C318" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="D318" s="22" t="s">
-        <v>1669</v>
+      <c r="D318" s="28" t="s">
+        <v>1667</v>
       </c>
       <c r="E318" t="s">
         <v>1370</v>
@@ -30544,8 +30622,8 @@
       <c r="C319" s="3" t="s">
         <v>779</v>
       </c>
-      <c r="D319" s="22" t="s">
-        <v>1508</v>
+      <c r="D319" s="28" t="s">
+        <v>1506</v>
       </c>
       <c r="E319" t="s">
         <v>1258</v>
@@ -30565,8 +30643,8 @@
       <c r="C320" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D320" s="22" t="s">
-        <v>1665</v>
+      <c r="D320" s="28" t="s">
+        <v>1663</v>
       </c>
       <c r="E320" t="s">
         <v>1284</v>
@@ -30585,8 +30663,8 @@
       <c r="C321" s="3" t="s">
         <v>895</v>
       </c>
-      <c r="D321" s="22" t="s">
-        <v>1673</v>
+      <c r="D321" s="28" t="s">
+        <v>1671</v>
       </c>
       <c r="E321" t="s">
         <v>1373</v>
@@ -30605,8 +30683,8 @@
       <c r="C322" t="s">
         <v>149</v>
       </c>
-      <c r="D322" s="17" t="s">
-        <v>1477</v>
+      <c r="D322" s="25" t="s">
+        <v>1476</v>
       </c>
       <c r="E322" t="s">
         <v>15</v>
@@ -30625,8 +30703,8 @@
       <c r="C323" t="s">
         <v>785</v>
       </c>
-      <c r="D323" s="17" t="s">
-        <v>1606</v>
+      <c r="D323" s="25" t="s">
+        <v>1604</v>
       </c>
       <c r="E323" t="s">
         <v>1257</v>
@@ -30645,8 +30723,8 @@
       <c r="C324" t="s">
         <v>786</v>
       </c>
-      <c r="D324" s="17" t="s">
-        <v>1671</v>
+      <c r="D324" s="25" t="s">
+        <v>1669</v>
       </c>
       <c r="E324" t="s">
         <v>1372</v>
@@ -30665,8 +30743,8 @@
       <c r="C325" t="s">
         <v>173</v>
       </c>
-      <c r="D325" s="17" t="s">
-        <v>1498</v>
+      <c r="D325" s="25" t="s">
+        <v>1496</v>
       </c>
       <c r="E325" t="s">
         <v>48</v>
@@ -30685,8 +30763,8 @@
       <c r="C326" t="s">
         <v>783</v>
       </c>
-      <c r="D326" s="17" t="s">
-        <v>1669</v>
+      <c r="D326" s="25" t="s">
+        <v>1667</v>
       </c>
       <c r="E326" t="s">
         <v>1370</v>
@@ -30703,8 +30781,8 @@
       <c r="C327" s="9" t="s">
         <v>880</v>
       </c>
-      <c r="D327" s="21" t="s">
-        <v>1674</v>
+      <c r="D327" s="26" t="s">
+        <v>1672</v>
       </c>
       <c r="E327" t="s">
         <v>1374</v>
@@ -30723,8 +30801,8 @@
       <c r="C328" t="s">
         <v>761</v>
       </c>
-      <c r="D328" s="17" t="s">
-        <v>1661</v>
+      <c r="D328" s="25" t="s">
+        <v>1659</v>
       </c>
       <c r="E328" t="s">
         <v>1365</v>
@@ -30738,8 +30816,8 @@
       <c r="C329" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="D329" s="22" t="s">
-        <v>1658</v>
+      <c r="D329" s="28" t="s">
+        <v>1656</v>
       </c>
       <c r="E329" t="s">
         <v>1358</v>
@@ -30755,7 +30833,7 @@
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
-      <c r="D330" s="22"/>
+      <c r="D330" s="28"/>
       <c r="G330" s="3"/>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.25">
@@ -30764,7 +30842,7 @@
       </c>
       <c r="B331" s="10"/>
       <c r="C331" s="3"/>
-      <c r="D331" s="22"/>
+      <c r="D331" s="28"/>
       <c r="G331" s="3"/>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
@@ -30775,8 +30853,8 @@
       <c r="C332" s="3" t="s">
         <v>789</v>
       </c>
-      <c r="D332" s="22" t="s">
-        <v>1675</v>
+      <c r="D332" s="28" t="s">
+        <v>1673</v>
       </c>
       <c r="E332" t="s">
         <v>1375</v>
@@ -30796,8 +30874,8 @@
       <c r="C333" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D333" s="20" t="s">
-        <v>1477</v>
+      <c r="D333" s="32" t="s">
+        <v>1476</v>
       </c>
       <c r="E333" t="s">
         <v>15</v>
@@ -30811,8 +30889,8 @@
       <c r="C334" s="9" t="s">
         <v>1424</v>
       </c>
-      <c r="D334" s="21" t="s">
-        <v>1652</v>
+      <c r="D334" s="26" t="s">
+        <v>1650</v>
       </c>
       <c r="E334" s="14" t="s">
         <v>1432</v>
@@ -30826,7 +30904,7 @@
       <c r="C335" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="D335" s="21" t="s">
+      <c r="D335" s="26" t="s">
         <v>1464</v>
       </c>
       <c r="E335" t="s">
@@ -30847,8 +30925,8 @@
       <c r="C336" s="9" t="s">
         <v>791</v>
       </c>
-      <c r="D336" s="21" t="s">
-        <v>1676</v>
+      <c r="D336" s="26" t="s">
+        <v>1674</v>
       </c>
       <c r="E336" t="s">
         <v>1376</v>
@@ -30868,8 +30946,8 @@
       <c r="C337" s="9" t="s">
         <v>793</v>
       </c>
-      <c r="D337" s="21" t="s">
-        <v>1677</v>
+      <c r="D337" s="26" t="s">
+        <v>1675</v>
       </c>
       <c r="E337" t="s">
         <v>1377</v>
@@ -30889,8 +30967,8 @@
       <c r="C338" s="9" t="s">
         <v>795</v>
       </c>
-      <c r="D338" s="21" t="s">
-        <v>1678</v>
+      <c r="D338" s="26" t="s">
+        <v>1676</v>
       </c>
       <c r="E338" t="s">
         <v>1378</v>
@@ -30910,8 +30988,8 @@
       <c r="C339" s="9" t="s">
         <v>797</v>
       </c>
-      <c r="D339" s="21" t="s">
-        <v>1679</v>
+      <c r="D339" s="26" t="s">
+        <v>1677</v>
       </c>
       <c r="E339" t="s">
         <v>1379</v>
@@ -30931,8 +31009,8 @@
       <c r="C340" s="9" t="s">
         <v>799</v>
       </c>
-      <c r="D340" s="21" t="s">
-        <v>1680</v>
+      <c r="D340" s="26" t="s">
+        <v>1678</v>
       </c>
       <c r="E340" t="s">
         <v>1380</v>
@@ -30952,8 +31030,8 @@
       <c r="C341" s="9" t="s">
         <v>801</v>
       </c>
-      <c r="D341" s="21" t="s">
-        <v>1681</v>
+      <c r="D341" s="26" t="s">
+        <v>1679</v>
       </c>
       <c r="E341" t="s">
         <v>1381</v>
@@ -30973,8 +31051,8 @@
       <c r="C342" s="9" t="s">
         <v>803</v>
       </c>
-      <c r="D342" s="21" t="s">
-        <v>1682</v>
+      <c r="D342" s="26" t="s">
+        <v>1680</v>
       </c>
       <c r="E342" t="s">
         <v>1382</v>
@@ -30994,8 +31072,8 @@
       <c r="C343" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="D343" s="21" t="s">
-        <v>1671</v>
+      <c r="D343" s="26" t="s">
+        <v>1669</v>
       </c>
       <c r="E343" t="s">
         <v>1383</v>
@@ -31014,8 +31092,8 @@
       <c r="C344" s="9" t="s">
         <v>776</v>
       </c>
-      <c r="D344" s="21" t="s">
-        <v>1661</v>
+      <c r="D344" s="26" t="s">
+        <v>1659</v>
       </c>
       <c r="E344" s="14" t="s">
         <v>1365</v>
@@ -31028,8 +31106,8 @@
       <c r="C345" s="9" t="s">
         <v>556</v>
       </c>
-      <c r="D345" s="21" t="s">
-        <v>1526</v>
+      <c r="D345" s="26" t="s">
+        <v>1524</v>
       </c>
       <c r="E345" s="14" t="s">
         <v>1265</v>
@@ -31042,8 +31120,8 @@
       <c r="C346" s="9" t="s">
         <v>771</v>
       </c>
-      <c r="D346" s="21" t="s">
-        <v>1658</v>
+      <c r="D346" s="26" t="s">
+        <v>1656</v>
       </c>
       <c r="E346" s="14" t="s">
         <v>1360</v>
@@ -31056,8 +31134,8 @@
       <c r="C347" t="s">
         <v>556</v>
       </c>
-      <c r="D347" s="17" t="s">
-        <v>1526</v>
+      <c r="D347" s="25" t="s">
+        <v>1524</v>
       </c>
       <c r="E347" s="14" t="s">
         <v>1265</v>
@@ -31071,8 +31149,8 @@
       <c r="C348" s="9" t="s">
         <v>807</v>
       </c>
-      <c r="D348" s="21" t="s">
-        <v>1683</v>
+      <c r="D348" s="26" t="s">
+        <v>1681</v>
       </c>
       <c r="E348" t="s">
         <v>1384</v>
@@ -31092,8 +31170,8 @@
       <c r="C349" s="9" t="s">
         <v>809</v>
       </c>
-      <c r="D349" s="21" t="s">
-        <v>1684</v>
+      <c r="D349" s="26" t="s">
+        <v>1682</v>
       </c>
       <c r="E349" t="s">
         <v>1350</v>
@@ -31113,8 +31191,8 @@
       <c r="C350" s="9" t="s">
         <v>810</v>
       </c>
-      <c r="D350" s="21" t="s">
-        <v>1685</v>
+      <c r="D350" s="26" t="s">
+        <v>1683</v>
       </c>
       <c r="E350" t="s">
         <v>1385</v>
@@ -31131,13 +31209,13 @@
         <v>78</v>
       </c>
       <c r="B351" s="9" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="C351" s="9" t="s">
         <v>1427</v>
       </c>
-      <c r="D351" s="21" t="s">
-        <v>1686</v>
+      <c r="D351" s="26" t="s">
+        <v>1684</v>
       </c>
       <c r="E351" t="s">
         <v>1429</v>
@@ -31157,8 +31235,8 @@
       <c r="C352" s="9" t="s">
         <v>1425</v>
       </c>
-      <c r="D352" s="21" t="s">
-        <v>1687</v>
+      <c r="D352" s="26" t="s">
+        <v>1685</v>
       </c>
       <c r="E352" t="s">
         <v>1430</v>
@@ -31173,8 +31251,8 @@
       <c r="C353" s="9" t="s">
         <v>1426</v>
       </c>
-      <c r="D353" s="21" t="s">
-        <v>1688</v>
+      <c r="D353" s="26" t="s">
+        <v>1686</v>
       </c>
       <c r="E353" t="s">
         <v>1431</v>
@@ -31191,8 +31269,8 @@
       <c r="C354" s="9" t="s">
         <v>1427</v>
       </c>
-      <c r="D354" s="21" t="s">
-        <v>1689</v>
+      <c r="D354" s="26" t="s">
+        <v>1687</v>
       </c>
       <c r="E354" t="s">
         <v>1429</v>
@@ -31212,8 +31290,8 @@
       <c r="C355" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="D355" s="21" t="s">
-        <v>1663</v>
+      <c r="D355" s="26" t="s">
+        <v>1661</v>
       </c>
       <c r="E355" t="s">
         <v>1237</v>
@@ -31233,8 +31311,8 @@
       <c r="C356" s="9" t="s">
         <v>813</v>
       </c>
-      <c r="D356" s="21" t="s">
-        <v>1690</v>
+      <c r="D356" s="26" t="s">
+        <v>1688</v>
       </c>
       <c r="E356" t="s">
         <v>1386</v>
@@ -31254,8 +31332,8 @@
       <c r="C357" s="9" t="s">
         <v>815</v>
       </c>
-      <c r="D357" s="21" t="s">
-        <v>1691</v>
+      <c r="D357" s="26" t="s">
+        <v>1689</v>
       </c>
       <c r="E357" t="s">
         <v>1387</v>
@@ -31275,8 +31353,8 @@
       <c r="C358" s="9" t="s">
         <v>817</v>
       </c>
-      <c r="D358" s="21" t="s">
-        <v>1692</v>
+      <c r="D358" s="26" t="s">
+        <v>1690</v>
       </c>
       <c r="E358" t="s">
         <v>1388</v>
@@ -31296,8 +31374,8 @@
       <c r="C359" s="9" t="s">
         <v>819</v>
       </c>
-      <c r="D359" s="21" t="s">
-        <v>1693</v>
+      <c r="D359" s="26" t="s">
+        <v>1691</v>
       </c>
       <c r="E359" t="s">
         <v>1389</v>
@@ -31311,11 +31389,11 @@
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C360" s="9"/>
-      <c r="D360" s="21"/>
+      <c r="D360" s="26"/>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A361" s="32" t="s">
-        <v>1729</v>
+      <c r="A361" s="22" t="s">
+        <v>1727</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
@@ -31323,70 +31401,81 @@
         <v>0</v>
       </c>
       <c r="C362" t="s">
-        <v>1703</v>
-      </c>
-      <c r="D362" s="28"/>
+        <v>1701</v>
+      </c>
+      <c r="D362" t="s">
+        <v>1740</v>
+      </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="C363" t="s">
         <v>1460</v>
       </c>
-      <c r="D363" s="28"/>
+      <c r="D363" t="s">
+        <v>1539</v>
+      </c>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="C364" t="s">
         <v>310</v>
       </c>
-      <c r="D364" s="28"/>
+      <c r="D364" t="s">
+        <v>1661</v>
+      </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="C365" t="s">
-        <v>1708</v>
-      </c>
-      <c r="D365" s="28"/>
+        <v>1706</v>
+      </c>
+      <c r="D365" t="s">
+        <v>1741</v>
+      </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="C366" t="s">
         <v>330</v>
       </c>
-      <c r="D366" s="28"/>
+      <c r="D366" t="s">
+        <v>1485</v>
+      </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="C367" t="s">
-        <v>1707</v>
-      </c>
-      <c r="D367" s="28"/>
+        <v>1705</v>
+      </c>
+      <c r="D367" t="s">
+        <v>1742</v>
+      </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="C368" t="s">
-        <v>1706</v>
-      </c>
-      <c r="D368" s="28"/>
-    </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D369" s="28"/>
+        <v>1704</v>
+      </c>
+      <c r="D368" t="s">
+        <v>1743</v>
+      </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -31394,84 +31483,102 @@
         <v>0</v>
       </c>
       <c r="B371" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="C371" t="s">
-        <v>1713</v>
-      </c>
-      <c r="D371" s="28"/>
+        <v>1711</v>
+      </c>
+      <c r="D371" t="s">
+        <v>1744</v>
+      </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="C372" t="s">
-        <v>1715</v>
-      </c>
-      <c r="D372" s="28"/>
+        <v>1713</v>
+      </c>
+      <c r="D372" t="s">
+        <v>1745</v>
+      </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="C373" t="s">
-        <v>1717</v>
-      </c>
-      <c r="D373" s="28"/>
+        <v>1715</v>
+      </c>
+      <c r="D373" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="C374" t="s">
         <v>346</v>
       </c>
-      <c r="D374" s="28"/>
+      <c r="D374" t="s">
+        <v>1531</v>
+      </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="C375" t="s">
-        <v>1720</v>
-      </c>
-      <c r="D375" s="28"/>
+        <v>1718</v>
+      </c>
+      <c r="D375" t="s">
+        <v>1746</v>
+      </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>102</v>
       </c>
       <c r="C376" t="s">
-        <v>1721</v>
-      </c>
-      <c r="D376" s="28"/>
+        <v>1719</v>
+      </c>
+      <c r="D376" t="s">
+        <v>1747</v>
+      </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>76</v>
       </c>
       <c r="C377" t="s">
-        <v>1722</v>
-      </c>
-      <c r="D377" s="28"/>
+        <v>1720</v>
+      </c>
+      <c r="D377" t="s">
+        <v>1748</v>
+      </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="C378" t="s">
-        <v>1724</v>
-      </c>
-      <c r="D378" s="28"/>
+        <v>1722</v>
+      </c>
+      <c r="D378" t="s">
+        <v>1749</v>
+      </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="C379" t="s">
-        <v>1726</v>
-      </c>
-      <c r="D379" s="28"/>
+        <v>1724</v>
+      </c>
+      <c r="D379" t="s">
+        <v>1750</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A146:XFD214">

</xml_diff>